<commit_message>
change background to solid color per request, removetext-shawdow comes from default, move youtube links from intubation to handlebar and label it from youtube
</commit_message>
<xml_diff>
--- a/neonatal/neonatal.xlsx
+++ b/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="760" windowWidth="23760" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="532">
   <si>
     <t>type</t>
   </si>
@@ -1469,12 +1469,6 @@
   </si>
   <si>
     <t>&lt;h2&gt;Intubation Video&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="http://www.youtube.com/watch?v=0VGiBwyfuNI"&gt;Intubation Video 1&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="http://www.youtube.com/watch?v=6PjvTsxwX5k"&gt;Intubation Video 2&lt;/a&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Enter weight (kg):&lt;/p&gt;</t>
@@ -2423,7 +2417,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2491,11 +2485,9 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="243" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="244" applyAlignment="1"/>
     <xf numFmtId="20" fontId="6" fillId="5" borderId="0" xfId="244" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="244" applyFill="1" applyAlignment="1">
@@ -3278,11 +3270,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J194"/>
+  <dimension ref="A1:J192"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3348,21 +3340,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="35" customFormat="1" ht="15">
+    <row r="4" spans="1:10" s="33" customFormat="1" ht="15">
       <c r="A4" s="12"/>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="31" t="s">
         <v>368</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31" t="s">
         <v>369</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" ht="12">
       <c r="A5" s="12"/>
@@ -3380,7 +3372,7 @@
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>372</v>
@@ -3460,1208 +3452,1203 @@
     </row>
     <row r="12" spans="1:10" ht="12">
       <c r="A12" s="7"/>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="27" t="s">
-        <v>413</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="B12" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:10" ht="12">
-      <c r="A13" s="16"/>
-      <c r="B13" t="s">
+    <row r="13" spans="1:10" s="12" customFormat="1" ht="12">
+      <c r="A13" s="7"/>
+      <c r="B13" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="12" customFormat="1" ht="12">
+      <c r="A14" s="7"/>
+      <c r="B14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="29" t="s">
-        <v>414</v>
-      </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:10" ht="12">
-      <c r="A14" s="7"/>
-      <c r="B14" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="D14" s="12" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="15" spans="1:10" s="12" customFormat="1" ht="12">
       <c r="A15" s="7"/>
-      <c r="B15" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="4" t="s">
-        <v>381</v>
+      <c r="B15" s="26" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="12" customFormat="1" ht="12">
       <c r="A16" s="7"/>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="12" customFormat="1" ht="13" customHeight="1">
+      <c r="A17" s="7"/>
+      <c r="B17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="12" customFormat="1" ht="12">
-      <c r="A17" s="7"/>
-      <c r="B17" s="26" t="s">
-        <v>15</v>
+      <c r="D17"/>
+      <c r="I17" s="12" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="12" customFormat="1" ht="12">
       <c r="A18" s="7"/>
-      <c r="B18" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="4" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="12" customFormat="1" ht="13" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="12" t="s">
+      <c r="B18" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15">
+      <c r="A19" s="16"/>
+      <c r="B19" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+    </row>
+    <row r="21" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A21" s="35"/>
+      <c r="B21" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" ht="15">
+      <c r="B22" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:10" ht="15">
+      <c r="A23" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:10" ht="12">
+      <c r="A24" s="12"/>
+      <c r="B24" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A25" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>436</v>
+      </c>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38" t="s">
+        <v>487</v>
+      </c>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A26" s="7"/>
+      <c r="B26" s="38" t="s">
+        <v>437</v>
+      </c>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38" t="s">
+        <v>488</v>
+      </c>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A28" s="39"/>
+      <c r="B28" t="s">
+        <v>439</v>
+      </c>
+      <c r="C28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" t="s">
+        <v>433</v>
+      </c>
+      <c r="E28"/>
+      <c r="F28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="24">
+      <c r="A29" s="7"/>
+      <c r="B29" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="18" customHeight="1">
+      <c r="A30" s="7"/>
+      <c r="B30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D19"/>
-      <c r="I19" s="12" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="12" customFormat="1" ht="12">
-      <c r="A20" s="7"/>
-      <c r="B20" s="26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="16"/>
-      <c r="B21" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-    </row>
-    <row r="23" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A23" s="37"/>
-      <c r="B23" s="14" t="s">
-        <v>425</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>430</v>
-      </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" ht="15">
-      <c r="B24" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15" t="s">
-        <v>429</v>
-      </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="1:10" ht="15">
-      <c r="A25" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="1:10" ht="12">
-      <c r="A26" s="12"/>
-      <c r="B26" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A27" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>438</v>
-      </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40" t="s">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="I30" t="s">
         <v>489</v>
       </c>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-    </row>
-    <row r="28" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="40" t="s">
-        <v>439</v>
-      </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40" t="s">
-        <v>490</v>
-      </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-    </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="41"/>
-      <c r="B29" s="13" t="s">
-        <v>440</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-    </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="41"/>
-      <c r="B30" t="s">
-        <v>441</v>
-      </c>
-      <c r="C30" t="s">
-        <v>149</v>
-      </c>
-      <c r="D30" t="s">
-        <v>435</v>
-      </c>
-      <c r="E30"/>
-      <c r="F30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="24">
+    </row>
+    <row r="31" spans="1:10" ht="18" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>321</v>
-      </c>
+        <v>444</v>
+      </c>
+      <c r="C31" s="19"/>
       <c r="D31" s="2" t="s">
-        <v>155</v>
+        <v>445</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="F31" s="2"/>
-      <c r="G31" t="s">
-        <v>444</v>
-      </c>
     </row>
     <row r="32" spans="1:10" ht="18" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>444</v>
+      </c>
+      <c r="C32" s="19"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="F32" s="2"/>
       <c r="I32" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15">
+      <c r="A33" s="7"/>
+      <c r="B33" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:9" s="12" customFormat="1" ht="15">
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+    </row>
+    <row r="35" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B35" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15" t="s">
+        <v>490</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+    </row>
+    <row r="36" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="18" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" ht="18" customHeight="1">
-      <c r="A34" s="7"/>
-      <c r="B34" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="F34" s="2"/>
-      <c r="I34" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="1:9" s="12" customFormat="1" ht="15">
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B37" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
+      <c r="A37" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B38" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15" t="s">
-        <v>493</v>
-      </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
+      <c r="A38" s="16"/>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="40"/>
+      <c r="F38" t="s">
+        <v>58</v>
+      </c>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A39" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="12.75" customHeight="1">
       <c r="A40" s="16"/>
       <c r="B40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>86</v>
-      </c>
-      <c r="E40" s="42"/>
-      <c r="F40" t="s">
-        <v>58</v>
-      </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="41" spans="1:9" ht="12.75" customHeight="1">
       <c r="A41" s="16"/>
-      <c r="B41" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" t="s">
-        <v>87</v>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="12.75" customHeight="1">
       <c r="A42" s="16"/>
-      <c r="B42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" t="s">
-        <v>60</v>
+      <c r="B42" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="12.75" customHeight="1">
       <c r="A43" s="16"/>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="D43" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1">
       <c r="A44" s="16"/>
-      <c r="B44" s="10" t="s">
-        <v>14</v>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>404</v>
       </c>
       <c r="E44" t="s">
-        <v>22</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:9" ht="12.75" customHeight="1">
       <c r="A45" s="16"/>
-      <c r="B45" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" t="s">
-        <v>415</v>
+      <c r="B45" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1">
       <c r="A46" s="16"/>
-      <c r="B46" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" t="s">
-        <v>404</v>
+      <c r="B46" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E46" t="s">
-        <v>25</v>
-      </c>
-      <c r="I46" s="9"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1">
       <c r="A47" s="16"/>
-      <c r="B47" s="11" t="s">
-        <v>15</v>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1">
       <c r="A48" s="16"/>
-      <c r="B48" s="10" t="s">
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>405</v>
+      </c>
+      <c r="E48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A49" s="16"/>
+      <c r="B49" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A50" s="16"/>
+      <c r="B50" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A51" s="16"/>
+      <c r="B51" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E48" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A49" s="16"/>
-      <c r="B49" t="s">
+      <c r="E51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A52" s="16"/>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A53" s="16"/>
+      <c r="B53" t="s">
         <v>23</v>
       </c>
-      <c r="C49" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A50" s="16"/>
-      <c r="B50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
-        <v>405</v>
-      </c>
-      <c r="E50" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A51" s="16"/>
-      <c r="B51" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A52" s="16"/>
-      <c r="B52" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A53" s="16"/>
-      <c r="B53" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E53" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="12.75" customHeight="1">
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="12.75" customHeight="1">
       <c r="A54" s="16"/>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>64</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="12.75" customHeight="1">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="12.75" customHeight="1">
       <c r="A55" s="16"/>
       <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>406</v>
+      </c>
+      <c r="E55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A56" s="16"/>
+      <c r="B56" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A57" s="16"/>
+      <c r="B57" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A58" s="16"/>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A59" s="16"/>
+      <c r="B59" t="s">
         <v>23</v>
       </c>
-      <c r="C55" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C59" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A56" s="16"/>
-      <c r="B56" t="s">
-        <v>23</v>
-      </c>
-      <c r="C56" t="s">
-        <v>64</v>
-      </c>
-      <c r="D56" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A57" s="16"/>
-      <c r="B57" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" t="s">
-        <v>406</v>
-      </c>
-      <c r="E57" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A58" s="16"/>
-      <c r="B58" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A59" s="16"/>
-      <c r="B59" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E59" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="12.75" customHeight="1">
+    <row r="60" spans="1:8" ht="12.75" customHeight="1">
       <c r="A60" s="16"/>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="C60" t="s">
+        <v>69</v>
       </c>
       <c r="D60" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="12.75" customHeight="1">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="12.75" customHeight="1">
       <c r="A61" s="16"/>
       <c r="B61" t="s">
-        <v>23</v>
-      </c>
-      <c r="C61" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="12.75" customHeight="1">
+        <v>407</v>
+      </c>
+      <c r="E61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="12.75" customHeight="1">
       <c r="A62" s="16"/>
-      <c r="B62" t="s">
-        <v>23</v>
-      </c>
-      <c r="C62" t="s">
-        <v>69</v>
-      </c>
-      <c r="D62" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A63" s="16"/>
-      <c r="B63" t="s">
+      <c r="B62" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A63" s="7"/>
+      <c r="B63" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+    </row>
+    <row r="64" spans="1:8" s="12" customFormat="1" ht="15">
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+    </row>
+    <row r="65" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B65" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+    </row>
+    <row r="66" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B66" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+    </row>
+    <row r="67" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A67" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+    </row>
+    <row r="68" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A68" s="16"/>
+      <c r="B68" t="s">
+        <v>503</v>
+      </c>
+      <c r="C68" t="s">
+        <v>504</v>
+      </c>
+      <c r="D68" t="s">
+        <v>502</v>
+      </c>
+      <c r="E68" s="40"/>
+      <c r="F68" t="s">
+        <v>58</v>
+      </c>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="69" spans="1:8" s="12" customFormat="1" ht="15">
+      <c r="A69" s="16"/>
+      <c r="B69" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
+      <c r="E69" t="s">
+        <v>510</v>
+      </c>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="30"/>
+    </row>
+    <row r="70" spans="1:8" s="12" customFormat="1" ht="15">
+      <c r="A70" s="16"/>
+      <c r="B70" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D63" t="s">
-        <v>407</v>
-      </c>
-      <c r="E63" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A64" s="16"/>
-      <c r="B64" s="18" t="s">
+      <c r="C70" s="30"/>
+      <c r="D70" s="41" t="s">
+        <v>507</v>
+      </c>
+      <c r="E70" s="30"/>
+      <c r="F70" s="30"/>
+      <c r="G70" s="30"/>
+      <c r="H70" s="30"/>
+    </row>
+    <row r="71" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A71" s="16"/>
+      <c r="B71" s="18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A65" s="7"/>
-      <c r="B65" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-    </row>
-    <row r="66" spans="1:8" s="12" customFormat="1" ht="15">
-      <c r="B66" s="32"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
-    </row>
-    <row r="67" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B67" s="14" t="s">
-        <v>498</v>
-      </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15" t="s">
-        <v>502</v>
-      </c>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-    </row>
-    <row r="68" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B68" s="14" t="s">
-        <v>499</v>
-      </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15" t="s">
-        <v>503</v>
-      </c>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="15"/>
-    </row>
-    <row r="69" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A69" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>500</v>
-      </c>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-    </row>
-    <row r="70" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A70" s="16"/>
-      <c r="B70" t="s">
-        <v>505</v>
-      </c>
-      <c r="C70" t="s">
-        <v>506</v>
-      </c>
-      <c r="D70" t="s">
-        <v>504</v>
-      </c>
-      <c r="E70" s="42"/>
-      <c r="F70" t="s">
-        <v>58</v>
-      </c>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-    </row>
-    <row r="71" spans="1:8" s="12" customFormat="1" ht="15">
-      <c r="A71" s="16"/>
-      <c r="B71" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" t="s">
-        <v>512</v>
-      </c>
-      <c r="F71" s="32"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="32"/>
     </row>
     <row r="72" spans="1:8" s="12" customFormat="1" ht="15">
       <c r="A72" s="16"/>
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="30"/>
+      <c r="D72" s="30"/>
+      <c r="E72" t="s">
+        <v>509</v>
+      </c>
+      <c r="F72" s="30"/>
+      <c r="G72" s="30"/>
+      <c r="H72" s="30"/>
+    </row>
+    <row r="73" spans="1:8" s="12" customFormat="1" ht="15">
+      <c r="A73" s="16"/>
+      <c r="B73" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="32"/>
-      <c r="D72" s="43" t="s">
-        <v>509</v>
-      </c>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="32"/>
-      <c r="H72" s="32"/>
-    </row>
-    <row r="73" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A73" s="16"/>
-      <c r="B73" s="18" t="s">
+      <c r="C73" s="30"/>
+      <c r="D73" s="41" t="s">
+        <v>508</v>
+      </c>
+      <c r="E73" s="30"/>
+      <c r="F73" s="30"/>
+      <c r="G73" s="30"/>
+      <c r="H73" s="30"/>
+    </row>
+    <row r="74" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A74" s="16"/>
+      <c r="B74" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="12" customFormat="1" ht="15">
-      <c r="A74" s="16"/>
-      <c r="B74" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" t="s">
+    <row r="75" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A75" s="7"/>
+      <c r="B75" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+    </row>
+    <row r="76" spans="1:8" s="12" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B76" s="30"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
+      <c r="H76" s="42"/>
+    </row>
+    <row r="77" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B77" s="14" t="s">
+        <v>512</v>
+      </c>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15" t="s">
+        <v>517</v>
+      </c>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+    </row>
+    <row r="78" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B78" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15" t="s">
+        <v>518</v>
+      </c>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+    </row>
+    <row r="79" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A79" s="7" t="s">
         <v>511</v>
       </c>
-      <c r="F74" s="32"/>
-      <c r="G74" s="32"/>
-      <c r="H74" s="32"/>
-    </row>
-    <row r="75" spans="1:8" s="12" customFormat="1" ht="15">
-      <c r="A75" s="16"/>
-      <c r="B75" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75" s="32"/>
-      <c r="D75" s="43" t="s">
-        <v>510</v>
-      </c>
-      <c r="E75" s="32"/>
-      <c r="F75" s="32"/>
-      <c r="G75" s="32"/>
-      <c r="H75" s="32"/>
-    </row>
-    <row r="76" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A76" s="16"/>
-      <c r="B76" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A77" s="7"/>
-      <c r="B77" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-    </row>
-    <row r="78" spans="1:8" s="12" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B78" s="32"/>
-      <c r="C78" s="44"/>
-      <c r="D78" s="44"/>
-      <c r="E78" s="44"/>
-      <c r="F78" s="44"/>
-      <c r="G78" s="44"/>
-      <c r="H78" s="44"/>
-    </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="8" t="s">
         <v>514</v>
       </c>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="15" t="s">
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+    </row>
+    <row r="80" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A80" s="16"/>
+      <c r="B80" t="s">
+        <v>515</v>
+      </c>
+      <c r="C80" t="s">
         <v>519</v>
       </c>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15"/>
-    </row>
-    <row r="80" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B80" s="14" t="s">
-        <v>515</v>
-      </c>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15" t="s">
-        <v>520</v>
-      </c>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
-      <c r="H80" s="15"/>
-    </row>
-    <row r="81" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A81" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>516</v>
-      </c>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-    </row>
-    <row r="82" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A82" s="16"/>
+      <c r="D80" t="s">
+        <v>435</v>
+      </c>
+      <c r="E80" s="40"/>
+      <c r="F80" t="s">
+        <v>58</v>
+      </c>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+    </row>
+    <row r="81" spans="1:8" ht="12">
+      <c r="A81" s="7"/>
+      <c r="B81" s="43" t="s">
+        <v>387</v>
+      </c>
+      <c r="C81" s="43" t="s">
+        <v>448</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="11" customHeight="1">
+      <c r="A82" s="7"/>
       <c r="B82" t="s">
-        <v>517</v>
+        <v>449</v>
       </c>
       <c r="C82" t="s">
-        <v>521</v>
+        <v>156</v>
       </c>
       <c r="D82" t="s">
-        <v>437</v>
-      </c>
-      <c r="E82" s="42"/>
+        <v>450</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>451</v>
+      </c>
       <c r="F82" t="s">
-        <v>58</v>
-      </c>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-    </row>
-    <row r="83" spans="1:8" ht="12">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="11" customHeight="1">
       <c r="A83" s="7"/>
-      <c r="B83" s="45" t="s">
-        <v>387</v>
-      </c>
-      <c r="C83" s="45" t="s">
-        <v>450</v>
+      <c r="B83" t="s">
+        <v>453</v>
+      </c>
+      <c r="C83" t="s">
+        <v>167</v>
+      </c>
+      <c r="D83" t="s">
+        <v>454</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>525</v>
+        <v>455</v>
+      </c>
+      <c r="F83" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="11" customHeight="1">
       <c r="A84" s="7"/>
       <c r="B84" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="C84" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="D84" t="s">
+        <v>457</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F84" t="s">
         <v>452</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="F84" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="11" customHeight="1">
       <c r="A85" s="7"/>
       <c r="B85" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="C85" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="D85" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="F85" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="11" customHeight="1">
       <c r="A86" s="7"/>
       <c r="B86" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="C86" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="D86" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="F86" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="11" customHeight="1">
       <c r="A87" s="7"/>
       <c r="B87" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="C87" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="D87" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="F87" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="11" customHeight="1">
       <c r="A88" s="7"/>
       <c r="B88" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="C88" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="D88" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="F88" t="s">
-        <v>454</v>
+        <v>470</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="11" customHeight="1">
       <c r="A89" s="7"/>
       <c r="B89" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="C89" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="D89" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="F89" t="s">
-        <v>454</v>
+        <v>473</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="11" customHeight="1">
       <c r="A90" s="7"/>
       <c r="B90" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="C90" t="s">
-        <v>232</v>
+        <v>260</v>
       </c>
       <c r="D90" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="11" customHeight="1">
       <c r="A91" s="7"/>
       <c r="B91" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C91" t="s">
-        <v>247</v>
+        <v>275</v>
       </c>
       <c r="D91" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="11" customHeight="1">
       <c r="A92" s="7"/>
       <c r="B92" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="C92" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
       <c r="D92" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="11" customHeight="1">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="12" customHeight="1">
       <c r="A93" s="7"/>
       <c r="B93" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="C93" t="s">
-        <v>275</v>
+        <v>303</v>
       </c>
       <c r="D93" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="11" customHeight="1">
-      <c r="A94" s="7"/>
-      <c r="B94" t="s">
-        <v>482</v>
-      </c>
-      <c r="C94" t="s">
-        <v>288</v>
-      </c>
-      <c r="D94" t="s">
-        <v>483</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="12" customHeight="1">
-      <c r="A95" s="7"/>
-      <c r="B95" t="s">
         <v>485</v>
       </c>
-      <c r="C95" t="s">
-        <v>303</v>
-      </c>
-      <c r="D95" t="s">
-        <v>486</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>487</v>
-      </c>
+    </row>
+    <row r="94" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A94" s="16"/>
+      <c r="E94" s="40"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
+    </row>
+    <row r="95" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A95" s="16"/>
+      <c r="E95" s="40"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
     </row>
     <row r="96" spans="1:8" ht="12.75" customHeight="1">
       <c r="A96" s="16"/>
-      <c r="E96" s="42"/>
+      <c r="E96" s="40"/>
       <c r="G96" s="9"/>
       <c r="H96" s="9"/>
     </row>
     <row r="97" spans="1:9" ht="12.75" customHeight="1">
       <c r="A97" s="16"/>
-      <c r="E97" s="42"/>
+      <c r="E97" s="40"/>
       <c r="G97" s="9"/>
       <c r="H97" s="9"/>
     </row>
     <row r="98" spans="1:9" ht="12.75" customHeight="1">
       <c r="A98" s="16"/>
-      <c r="E98" s="42"/>
+      <c r="E98" s="40"/>
       <c r="G98" s="9"/>
       <c r="H98" s="9"/>
     </row>
     <row r="99" spans="1:9" ht="12.75" customHeight="1">
       <c r="A99" s="16"/>
-      <c r="E99" s="42"/>
+      <c r="E99" s="40"/>
       <c r="G99" s="9"/>
       <c r="H99" s="9"/>
     </row>
-    <row r="100" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A100" s="16"/>
-      <c r="E100" s="42"/>
-      <c r="G100" s="9"/>
-      <c r="H100" s="9"/>
-    </row>
-    <row r="101" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A101" s="16"/>
-      <c r="E101" s="42"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="9"/>
+    <row r="100" spans="1:9" ht="12">
+      <c r="A100" s="7"/>
+      <c r="B100" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E100" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="24">
+      <c r="A101" s="7"/>
+      <c r="B101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="102" spans="1:9" ht="12">
       <c r="A102" s="7"/>
-      <c r="B102" s="10" t="s">
+      <c r="B102" t="s">
+        <v>21</v>
+      </c>
+      <c r="C102" t="s">
+        <v>16</v>
+      </c>
+      <c r="F102" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="12">
+      <c r="A103" s="7"/>
+      <c r="B103" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E102" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="24">
-      <c r="A103" s="7"/>
-      <c r="B103" t="s">
-        <v>4</v>
-      </c>
-      <c r="D103" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="12">
+      <c r="E103" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="24">
       <c r="A104" s="7"/>
       <c r="B104" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C104" t="s">
-        <v>16</v>
-      </c>
-      <c r="F104" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="12">
+        <v>24</v>
+      </c>
+      <c r="D104" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="12.75" customHeight="1">
       <c r="A105" s="7"/>
-      <c r="B105" s="10" t="s">
-        <v>14</v>
+      <c r="B105" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" t="s">
+        <v>404</v>
       </c>
       <c r="E105" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="24">
+        <v>25</v>
+      </c>
+      <c r="I105" s="9"/>
+    </row>
+    <row r="106" spans="1:9" ht="12.75" customHeight="1">
       <c r="A106" s="7"/>
-      <c r="B106" t="s">
-        <v>23</v>
-      </c>
-      <c r="C106" t="s">
-        <v>24</v>
-      </c>
-      <c r="D106" t="s">
-        <v>415</v>
+      <c r="B106" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="12.75" customHeight="1">
       <c r="A107" s="7"/>
-      <c r="B107" t="s">
-        <v>4</v>
-      </c>
-      <c r="D107" t="s">
-        <v>404</v>
+      <c r="B107" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E107" t="s">
-        <v>25</v>
-      </c>
-      <c r="I107" s="9"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="108" spans="1:9" ht="12.75" customHeight="1">
       <c r="A108" s="7"/>
-      <c r="B108" s="11" t="s">
-        <v>15</v>
+      <c r="B108" t="s">
+        <v>23</v>
+      </c>
+      <c r="C108" t="s">
+        <v>27</v>
+      </c>
+      <c r="D108" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="12.75" customHeight="1">
       <c r="A109" s="7"/>
-      <c r="B109" s="10" t="s">
-        <v>14</v>
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+      <c r="D109" t="s">
+        <v>405</v>
       </c>
       <c r="E109" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="12.75" customHeight="1">
       <c r="A110" s="7"/>
-      <c r="B110" t="s">
-        <v>23</v>
-      </c>
-      <c r="C110" t="s">
-        <v>27</v>
-      </c>
-      <c r="D110" t="s">
-        <v>416</v>
+      <c r="B110" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="12.75" customHeight="1">
       <c r="A111" s="7"/>
-      <c r="B111" t="s">
-        <v>4</v>
-      </c>
-      <c r="D111" t="s">
-        <v>405</v>
-      </c>
-      <c r="E111" t="s">
-        <v>32</v>
+      <c r="B111" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="12.75" customHeight="1">
       <c r="A112" s="7"/>
-      <c r="B112" s="11" t="s">
-        <v>15</v>
+      <c r="B112" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E112" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="12.75" customHeight="1">
       <c r="A113" s="7"/>
-      <c r="B113" s="11" t="s">
-        <v>15</v>
+      <c r="B113" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="114" spans="1:10" ht="12.75" customHeight="1">
       <c r="A114" s="7"/>
-      <c r="B114" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E114" t="s">
-        <v>524</v>
+      <c r="B114" t="s">
+        <v>41</v>
+      </c>
+      <c r="C114" t="s">
+        <v>48</v>
+      </c>
+      <c r="D114" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" customHeight="1">
       <c r="A115" s="7"/>
-      <c r="B115" s="12" t="s">
+      <c r="B115" t="s">
         <v>4</v>
       </c>
       <c r="D115" t="s">
-        <v>72</v>
+        <v>420</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="12.75" customHeight="1">
       <c r="A116" s="7"/>
       <c r="B116" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C116" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D116" t="s">
         <v>421</v>
@@ -4670,7 +4657,10 @@
     <row r="117" spans="1:10" ht="12.75" customHeight="1">
       <c r="A117" s="7"/>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="C117" t="s">
+        <v>44</v>
       </c>
       <c r="D117" t="s">
         <v>422</v>
@@ -4679,305 +4669,299 @@
     <row r="118" spans="1:10" ht="12.75" customHeight="1">
       <c r="A118" s="7"/>
       <c r="B118" t="s">
-        <v>42</v>
-      </c>
-      <c r="C118" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D118" t="s">
-        <v>423</v>
+        <v>408</v>
+      </c>
+      <c r="E118" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="12.75" customHeight="1">
       <c r="A119" s="7"/>
       <c r="B119" t="s">
-        <v>42</v>
-      </c>
-      <c r="C119" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D119" t="s">
-        <v>424</v>
+        <v>409</v>
+      </c>
+      <c r="E119" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="12.75" customHeight="1">
       <c r="A120" s="7"/>
-      <c r="B120" t="s">
-        <v>4</v>
-      </c>
-      <c r="D120" t="s">
-        <v>408</v>
-      </c>
-      <c r="E120" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" ht="12.75" customHeight="1">
+      <c r="B120" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="20" customHeight="1">
       <c r="A121" s="7"/>
-      <c r="B121" t="s">
-        <v>4</v>
-      </c>
-      <c r="D121" t="s">
-        <v>409</v>
-      </c>
-      <c r="E121" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A122" s="7"/>
-      <c r="B122" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" ht="20" customHeight="1">
-      <c r="A123" s="7"/>
-      <c r="B123" s="8" t="s">
-        <v>518</v>
-      </c>
-      <c r="C123" s="13"/>
-      <c r="D123" s="13"/>
-      <c r="E123" s="13"/>
-      <c r="F123" s="13"/>
-      <c r="G123" s="13"/>
-      <c r="H123" s="13"/>
-    </row>
-    <row r="124" spans="1:10" ht="15">
-      <c r="A124" s="16"/>
-      <c r="B124" s="8" t="s">
-        <v>428</v>
-      </c>
-      <c r="C124" s="30"/>
-      <c r="D124" s="31"/>
-      <c r="E124" s="30"/>
-      <c r="F124" s="30"/>
-    </row>
-    <row r="126" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A126" s="37"/>
-      <c r="B126" s="14" t="s">
+      <c r="B121" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="13"/>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+    </row>
+    <row r="122" spans="1:10" ht="15">
+      <c r="A122" s="16"/>
+      <c r="B122" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="C122" s="28"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="28"/>
+      <c r="F122" s="28"/>
+    </row>
+    <row r="124" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A124" s="35"/>
+      <c r="B124" s="14" t="s">
         <v>392</v>
       </c>
-      <c r="E126" s="15" t="s">
+      <c r="E124" s="15" t="s">
         <v>393</v>
       </c>
-      <c r="I126" s="3"/>
-      <c r="J126" s="3"/>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+    </row>
+    <row r="125" spans="1:10" ht="12.75" customHeight="1">
+      <c r="B125" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="F125" s="15"/>
+      <c r="G125" s="15"/>
+      <c r="H125" s="15"/>
+    </row>
+    <row r="126" spans="1:10" ht="15">
+      <c r="A126" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="13"/>
+      <c r="H126" s="13"/>
     </row>
     <row r="127" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B127" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="C127" s="15"/>
-      <c r="D127" s="15"/>
-      <c r="E127" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="F127" s="15"/>
-      <c r="G127" s="15"/>
-      <c r="H127" s="15"/>
-    </row>
-    <row r="128" spans="1:10" ht="15">
-      <c r="A128" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="B128" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C128" s="13"/>
-      <c r="D128" s="13"/>
-      <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
-      <c r="G128" s="13"/>
-      <c r="H128" s="13"/>
+      <c r="A127" s="7"/>
+      <c r="B127" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H127" s="3"/>
+    </row>
+    <row r="128" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A128" s="7"/>
+      <c r="B128" t="s">
+        <v>76</v>
+      </c>
+      <c r="C128" t="s">
+        <v>77</v>
+      </c>
+      <c r="F128" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="129" spans="1:9" ht="12.75" customHeight="1">
       <c r="A129" s="7"/>
       <c r="B129" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H129" s="3"/>
+      <c r="E129" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="130" spans="1:9" ht="12.75" customHeight="1">
       <c r="A130" s="7"/>
-      <c r="B130" t="s">
-        <v>76</v>
-      </c>
-      <c r="C130" t="s">
-        <v>77</v>
-      </c>
-      <c r="F130" t="s">
-        <v>13</v>
+      <c r="B130" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D130" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="12.75" customHeight="1">
       <c r="A131" s="7"/>
-      <c r="B131" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E131" t="s">
-        <v>78</v>
+      <c r="B131" t="s">
+        <v>4</v>
+      </c>
+      <c r="D131" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="12.75" customHeight="1">
       <c r="A132" s="7"/>
-      <c r="B132" s="4" t="s">
-        <v>4</v>
+      <c r="B132" t="s">
+        <v>23</v>
+      </c>
+      <c r="C132" t="s">
+        <v>116</v>
       </c>
       <c r="D132" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="12.75" customHeight="1">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="61" customHeight="1">
       <c r="A133" s="7"/>
       <c r="B133" t="s">
         <v>4</v>
       </c>
       <c r="D133" t="s">
-        <v>113</v>
+        <v>396</v>
+      </c>
+      <c r="E133" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="12.75" customHeight="1">
       <c r="A134" s="7"/>
       <c r="B134" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C134" t="s">
-        <v>116</v>
-      </c>
-      <c r="D134" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="61" customHeight="1">
+        <v>34</v>
+      </c>
+      <c r="I134" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="12.75" customHeight="1">
       <c r="A135" s="7"/>
-      <c r="B135" t="s">
-        <v>4</v>
-      </c>
-      <c r="D135" t="s">
-        <v>396</v>
-      </c>
-      <c r="E135" t="s">
-        <v>117</v>
+      <c r="B135" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="12.75" customHeight="1">
       <c r="A136" s="7"/>
-      <c r="B136" t="s">
-        <v>4</v>
-      </c>
-      <c r="C136" t="s">
-        <v>34</v>
-      </c>
-      <c r="I136" t="s">
-        <v>36</v>
+      <c r="B136" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E136" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="12.75" customHeight="1">
       <c r="A137" s="7"/>
-      <c r="B137" s="6" t="s">
-        <v>15</v>
+      <c r="B137" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D137" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="12.75" customHeight="1">
       <c r="A138" s="7"/>
-      <c r="B138" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E138" t="s">
-        <v>105</v>
+      <c r="B138" t="s">
+        <v>4</v>
+      </c>
+      <c r="D138" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="12.75" customHeight="1">
       <c r="A139" s="7"/>
-      <c r="B139" s="4" t="s">
-        <v>4</v>
+      <c r="B139" t="s">
+        <v>23</v>
+      </c>
+      <c r="C139" t="s">
+        <v>118</v>
       </c>
       <c r="D139" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="12.75" customHeight="1">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="75" customHeight="1">
       <c r="A140" s="7"/>
       <c r="B140" t="s">
         <v>4</v>
       </c>
       <c r="D140" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" ht="12.75" customHeight="1">
+        <v>397</v>
+      </c>
+      <c r="E140" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="36" customHeight="1">
       <c r="A141" s="7"/>
       <c r="B141" t="s">
-        <v>23</v>
-      </c>
-      <c r="C141" t="s">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="D141" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" ht="75" customHeight="1">
+        <v>398</v>
+      </c>
+      <c r="E141" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="41" customHeight="1">
       <c r="A142" s="7"/>
       <c r="B142" t="s">
         <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E142" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="36" customHeight="1">
+    <row r="143" spans="1:9" ht="12" customHeight="1">
       <c r="A143" s="7"/>
       <c r="B143" t="s">
         <v>4</v>
       </c>
-      <c r="D143" t="s">
-        <v>398</v>
-      </c>
-      <c r="E143" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" ht="41" customHeight="1">
+      <c r="C143" t="s">
+        <v>103</v>
+      </c>
+      <c r="I143" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="12.75" customHeight="1">
       <c r="A144" s="7"/>
-      <c r="B144" t="s">
-        <v>4</v>
-      </c>
-      <c r="D144" t="s">
-        <v>399</v>
-      </c>
-      <c r="E144" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" ht="12" customHeight="1">
+      <c r="B144" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="12.75" customHeight="1">
       <c r="A145" s="7"/>
-      <c r="B145" t="s">
-        <v>4</v>
-      </c>
-      <c r="C145" t="s">
-        <v>103</v>
-      </c>
-      <c r="I145" t="s">
-        <v>104</v>
+      <c r="B145" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E145" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="12.75" customHeight="1">
       <c r="A146" s="7"/>
-      <c r="B146" s="6" t="s">
-        <v>15</v>
+      <c r="B146" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" t="s">
+        <v>129</v>
+      </c>
+      <c r="I146" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="12.75" customHeight="1">
       <c r="A147" s="7"/>
-      <c r="B147" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E147" t="s">
-        <v>131</v>
+      <c r="B147" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="12.75" customHeight="1">
@@ -4985,11 +4969,8 @@
       <c r="B148" t="s">
         <v>4</v>
       </c>
-      <c r="C148" t="s">
-        <v>129</v>
-      </c>
-      <c r="I148" t="s">
-        <v>130</v>
+      <c r="D148" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="12.75" customHeight="1">
@@ -5000,347 +4981,353 @@
     </row>
     <row r="150" spans="1:9" ht="12.75" customHeight="1">
       <c r="A150" s="7"/>
-      <c r="B150" t="s">
-        <v>4</v>
-      </c>
-      <c r="D150" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A151" s="7"/>
-      <c r="B151" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A152" s="7"/>
-      <c r="B152" s="8" t="s">
+      <c r="B150" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C152" s="13"/>
-      <c r="D152" s="13"/>
-      <c r="E152" s="13"/>
-      <c r="F152" s="13"/>
-      <c r="G152" s="13"/>
-      <c r="H152" s="13"/>
-    </row>
-    <row r="154" spans="1:9" s="14" customFormat="1" ht="15">
-      <c r="A154" s="28"/>
-      <c r="B154" s="14" t="s">
+      <c r="C150" s="13"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="13"/>
+      <c r="G150" s="13"/>
+      <c r="H150" s="13"/>
+    </row>
+    <row r="152" spans="1:9" s="14" customFormat="1" ht="15">
+      <c r="A152" s="27"/>
+      <c r="B152" s="14" t="s">
         <v>400</v>
       </c>
-      <c r="C154" s="38"/>
-      <c r="D154" s="39"/>
-      <c r="E154" s="15" t="s">
+      <c r="C152" s="36"/>
+      <c r="D152" s="37"/>
+      <c r="E152" s="15" t="s">
         <v>401</v>
       </c>
-      <c r="F154" s="38"/>
-    </row>
-    <row r="155" spans="1:9" s="14" customFormat="1" ht="15">
-      <c r="A155" s="28"/>
-      <c r="B155" s="14" t="s">
+      <c r="F152" s="36"/>
+    </row>
+    <row r="153" spans="1:9" s="14" customFormat="1" ht="15">
+      <c r="A153" s="27"/>
+      <c r="B153" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="C155" s="38"/>
-      <c r="D155" s="39"/>
-      <c r="E155" s="15" t="s">
+      <c r="C153" s="36"/>
+      <c r="D153" s="37"/>
+      <c r="E153" s="15" t="s">
         <v>403</v>
       </c>
-      <c r="F155" s="38"/>
-    </row>
-    <row r="156" spans="1:9" ht="15">
-      <c r="A156" s="7" t="s">
-        <v>497</v>
-      </c>
-      <c r="B156" s="8" t="s">
+      <c r="F153" s="36"/>
+    </row>
+    <row r="154" spans="1:9" ht="15">
+      <c r="A154" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="B154" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
-      <c r="E156" s="8"/>
-      <c r="F156" s="8"/>
-      <c r="G156" s="8"/>
-      <c r="H156" s="8"/>
-    </row>
-    <row r="157" spans="1:9" ht="15">
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
+      <c r="F154" s="8"/>
+      <c r="G154" s="8"/>
+      <c r="H154" s="8"/>
+    </row>
+    <row r="155" spans="1:9" ht="15">
+      <c r="A155" s="7"/>
+      <c r="B155" t="s">
+        <v>55</v>
+      </c>
+      <c r="C155" t="s">
+        <v>56</v>
+      </c>
+      <c r="D155" t="s">
+        <v>57</v>
+      </c>
+      <c r="E155" s="30"/>
+      <c r="F155" t="s">
+        <v>58</v>
+      </c>
+      <c r="G155" s="9"/>
+      <c r="H155" s="9"/>
+    </row>
+    <row r="156" spans="1:9" ht="12">
+      <c r="A156" s="7"/>
+      <c r="B156" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E156" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="24">
       <c r="A157" s="7"/>
       <c r="B157" t="s">
-        <v>55</v>
-      </c>
-      <c r="C157" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="D157" t="s">
-        <v>57</v>
-      </c>
-      <c r="E157" s="32"/>
-      <c r="F157" t="s">
-        <v>58</v>
-      </c>
-      <c r="G157" s="9"/>
-      <c r="H157" s="9"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="158" spans="1:9" ht="12">
       <c r="A158" s="7"/>
-      <c r="B158" s="10" t="s">
+      <c r="B158" t="s">
+        <v>21</v>
+      </c>
+      <c r="C158" t="s">
+        <v>16</v>
+      </c>
+      <c r="F158" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="12">
+      <c r="A159" s="7"/>
+      <c r="B159" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E158" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" ht="24">
-      <c r="A159" s="7"/>
-      <c r="B159" t="s">
-        <v>4</v>
-      </c>
-      <c r="D159" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" ht="12">
+      <c r="E159" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="24">
       <c r="A160" s="7"/>
       <c r="B160" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C160" t="s">
-        <v>16</v>
-      </c>
-      <c r="F160" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" ht="12">
+        <v>24</v>
+      </c>
+      <c r="D160" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="12.75" customHeight="1">
       <c r="A161" s="7"/>
-      <c r="B161" s="10" t="s">
-        <v>14</v>
+      <c r="B161" t="s">
+        <v>4</v>
+      </c>
+      <c r="D161" t="s">
+        <v>404</v>
       </c>
       <c r="E161" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" ht="24">
+        <v>25</v>
+      </c>
+      <c r="I161" s="9"/>
+    </row>
+    <row r="162" spans="1:9" ht="12.75" customHeight="1">
       <c r="A162" s="7"/>
-      <c r="B162" t="s">
-        <v>23</v>
-      </c>
-      <c r="C162" t="s">
-        <v>24</v>
-      </c>
-      <c r="D162" t="s">
-        <v>415</v>
+      <c r="B162" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="12.75" customHeight="1">
       <c r="A163" s="7"/>
-      <c r="B163" t="s">
-        <v>4</v>
-      </c>
-      <c r="D163" t="s">
-        <v>404</v>
+      <c r="B163" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E163" t="s">
-        <v>25</v>
-      </c>
-      <c r="I163" s="9"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="164" spans="1:9" ht="12.75" customHeight="1">
       <c r="A164" s="7"/>
-      <c r="B164" s="11" t="s">
-        <v>15</v>
+      <c r="B164" t="s">
+        <v>23</v>
+      </c>
+      <c r="C164" t="s">
+        <v>27</v>
+      </c>
+      <c r="D164" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="12.75" customHeight="1">
       <c r="A165" s="7"/>
-      <c r="B165" s="10" t="s">
-        <v>14</v>
+      <c r="B165" t="s">
+        <v>4</v>
+      </c>
+      <c r="D165" t="s">
+        <v>405</v>
       </c>
       <c r="E165" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="12.75" customHeight="1">
       <c r="A166" s="7"/>
-      <c r="B166" t="s">
-        <v>23</v>
-      </c>
-      <c r="C166" t="s">
-        <v>27</v>
-      </c>
-      <c r="D166" t="s">
-        <v>416</v>
+      <c r="B166" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="12.75" customHeight="1">
       <c r="A167" s="7"/>
-      <c r="B167" t="s">
-        <v>4</v>
-      </c>
-      <c r="D167" t="s">
-        <v>405</v>
-      </c>
-      <c r="E167" t="s">
-        <v>32</v>
+      <c r="B167" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="12.75" customHeight="1">
       <c r="A168" s="7"/>
-      <c r="B168" s="11" t="s">
-        <v>15</v>
+      <c r="B168" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E168" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="12.75" customHeight="1">
       <c r="A169" s="7"/>
-      <c r="B169" s="11" t="s">
-        <v>15</v>
+      <c r="B169" t="s">
+        <v>4</v>
+      </c>
+      <c r="D169" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="12.75" customHeight="1">
       <c r="A170" s="7"/>
-      <c r="B170" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E170" t="s">
-        <v>61</v>
+      <c r="B170" t="s">
+        <v>23</v>
+      </c>
+      <c r="C170" t="s">
+        <v>63</v>
+      </c>
+      <c r="D170" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="12.75" customHeight="1">
       <c r="A171" s="7"/>
       <c r="B171" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="C171" t="s">
+        <v>64</v>
       </c>
       <c r="D171" t="s">
-        <v>62</v>
+        <v>416</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="12.75" customHeight="1">
       <c r="A172" s="7"/>
       <c r="B172" t="s">
-        <v>23</v>
-      </c>
-      <c r="C172" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="D172" t="s">
-        <v>417</v>
+        <v>406</v>
+      </c>
+      <c r="E172" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="12.75" customHeight="1">
       <c r="A173" s="7"/>
-      <c r="B173" t="s">
-        <v>23</v>
-      </c>
-      <c r="C173" t="s">
-        <v>64</v>
-      </c>
-      <c r="D173" t="s">
-        <v>418</v>
+      <c r="B173" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="12.75" customHeight="1">
       <c r="A174" s="7"/>
-      <c r="B174" t="s">
-        <v>4</v>
-      </c>
-      <c r="D174" t="s">
-        <v>406</v>
+      <c r="B174" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E174" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="12.75" customHeight="1">
       <c r="A175" s="7"/>
-      <c r="B175" s="11" t="s">
-        <v>15</v>
+      <c r="B175" t="s">
+        <v>4</v>
+      </c>
+      <c r="D175" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="12.75" customHeight="1">
       <c r="A176" s="7"/>
-      <c r="B176" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E176" t="s">
-        <v>66</v>
+      <c r="B176" t="s">
+        <v>23</v>
+      </c>
+      <c r="C176" t="s">
+        <v>68</v>
+      </c>
+      <c r="D176" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="12.75" customHeight="1">
       <c r="A177" s="7"/>
       <c r="B177" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="C177" t="s">
+        <v>69</v>
       </c>
       <c r="D177" t="s">
-        <v>67</v>
+        <v>418</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="12.75" customHeight="1">
       <c r="A178" s="7"/>
       <c r="B178" t="s">
-        <v>23</v>
-      </c>
-      <c r="C178" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D178" t="s">
-        <v>419</v>
+        <v>407</v>
+      </c>
+      <c r="E178" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="12.75" customHeight="1">
       <c r="A179" s="7"/>
-      <c r="B179" t="s">
-        <v>23</v>
-      </c>
-      <c r="C179" t="s">
-        <v>69</v>
-      </c>
-      <c r="D179" t="s">
-        <v>420</v>
+      <c r="B179" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="12.75" customHeight="1">
       <c r="A180" s="7"/>
-      <c r="B180" t="s">
-        <v>4</v>
-      </c>
-      <c r="D180" t="s">
-        <v>407</v>
+      <c r="B180" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E180" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="181" spans="1:8" ht="12.75" customHeight="1">
       <c r="A181" s="7"/>
-      <c r="B181" s="11" t="s">
-        <v>15</v>
+      <c r="B181" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D181" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="12.75" customHeight="1">
       <c r="A182" s="7"/>
-      <c r="B182" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E182" t="s">
-        <v>71</v>
+      <c r="B182" t="s">
+        <v>41</v>
+      </c>
+      <c r="C182" t="s">
+        <v>48</v>
+      </c>
+      <c r="D182" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="12.75" customHeight="1">
       <c r="A183" s="7"/>
-      <c r="B183" s="12" t="s">
+      <c r="B183" t="s">
         <v>4</v>
       </c>
       <c r="D183" t="s">
-        <v>72</v>
+        <v>420</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="12.75" customHeight="1">
       <c r="A184" s="7"/>
       <c r="B184" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C184" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D184" t="s">
         <v>421</v>
@@ -5349,7 +5336,10 @@
     <row r="185" spans="1:8" ht="12.75" customHeight="1">
       <c r="A185" s="7"/>
       <c r="B185" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="C185" t="s">
+        <v>44</v>
       </c>
       <c r="D185" t="s">
         <v>422</v>
@@ -5358,71 +5348,47 @@
     <row r="186" spans="1:8" ht="12.75" customHeight="1">
       <c r="A186" s="7"/>
       <c r="B186" t="s">
-        <v>42</v>
-      </c>
-      <c r="C186" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D186" t="s">
-        <v>423</v>
+        <v>408</v>
+      </c>
+      <c r="E186" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="12.75" customHeight="1">
       <c r="A187" s="7"/>
       <c r="B187" t="s">
-        <v>42</v>
-      </c>
-      <c r="C187" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D187" t="s">
-        <v>424</v>
+        <v>409</v>
+      </c>
+      <c r="E187" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="12.75" customHeight="1">
       <c r="A188" s="7"/>
-      <c r="B188" t="s">
-        <v>4</v>
-      </c>
-      <c r="D188" t="s">
-        <v>408</v>
-      </c>
-      <c r="E188" t="s">
-        <v>73</v>
+      <c r="B188" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="12.75" customHeight="1">
       <c r="A189" s="7"/>
-      <c r="B189" t="s">
-        <v>4</v>
-      </c>
-      <c r="D189" t="s">
-        <v>409</v>
-      </c>
-      <c r="E189" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A190" s="7"/>
-      <c r="B190" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A191" s="7"/>
-      <c r="B191" s="8" t="s">
+      <c r="B189" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C191" s="8"/>
-      <c r="D191" s="8"/>
-      <c r="E191" s="8"/>
-      <c r="F191" s="8"/>
-      <c r="G191" s="8"/>
-      <c r="H191" s="8"/>
-    </row>
-    <row r="194" spans="2:2" ht="12.75" customHeight="1">
-      <c r="B194" s="36" t="s">
+      <c r="C189" s="8"/>
+      <c r="D189" s="8"/>
+      <c r="E189" s="8"/>
+      <c r="F189" s="8"/>
+      <c r="G189" s="8"/>
+      <c r="H189" s="8"/>
+    </row>
+    <row r="192" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B192" s="34" t="s">
         <v>380</v>
       </c>
     </row>
@@ -5441,7 +5407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5469,7 +5435,7 @@
         <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
@@ -5480,7 +5446,7 @@
         <v>379</v>
       </c>
       <c r="D3" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
@@ -5491,7 +5457,7 @@
         <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
@@ -5502,7 +5468,7 @@
         <v>141</v>
       </c>
       <c r="D5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1">
@@ -5540,18 +5506,18 @@
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B11" t="s">
         <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1">
       <c r="A12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B12" t="s">
         <v>142</v>
@@ -5562,24 +5528,24 @@
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" t="s">
+        <v>430</v>
+      </c>
+      <c r="B14" t="s">
         <v>432</v>
       </c>
-      <c r="B14" t="s">
-        <v>434</v>
-      </c>
       <c r="C14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
@@ -5590,7 +5556,7 @@
         <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1">
@@ -5601,7 +5567,7 @@
         <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1">
@@ -5612,7 +5578,7 @@
         <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1">
@@ -5782,40 +5748,40 @@
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B39" t="s">
+        <v>505</v>
+      </c>
+      <c r="C39" t="s">
         <v>507</v>
-      </c>
-      <c r="C39" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
+        <v>504</v>
+      </c>
+      <c r="B40" t="s">
         <v>506</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>508</v>
-      </c>
-      <c r="C40" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B42" t="s">
         <v>153</v>
       </c>
       <c r="C42" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B43" t="s">
         <v>91</v>
@@ -5826,7 +5792,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
change in weight loss calculator: if weight gain show positive amount also say gain, when lost say lost
</commit_message>
<xml_diff>
--- a/neonatal/neonatal.xlsx
+++ b/neonatal/neonatal.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="540">
   <si>
     <t>type</t>
   </si>
@@ -1826,6 +1826,30 @@
   </si>
   <si>
     <t>img/CALCULATORS_ICON.png</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>data('birthW') &amp;&amp; data('currW')&amp;&amp;data('currW')-data('birthW')&lt;0</t>
+  </si>
+  <si>
+    <t>weightGain</t>
+  </si>
+  <si>
+    <t>data('currW')-data('birthW')</t>
+  </si>
+  <si>
+    <t>weightGainPerc</t>
+  </si>
+  <si>
+    <t>&lt;span style="background-color: yellow"&gt;&lt;b&gt;Baby Weight Gain:{{calculates.weightGain}}  g; {{calculates.weightGainPerc}} %&lt;/b&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>(calculates.weightGain()*100.0/data('birthW')).toFixed(2)</t>
+  </si>
+  <si>
+    <t>data('birthW') &amp;&amp; data('currW')&amp;&amp;data('currW')-data('birthW')&gt;=0</t>
   </si>
 </sst>
 </file>
@@ -3270,11 +3294,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J192"/>
+  <dimension ref="A1:J193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3315,6 +3339,9 @@
       <c r="I1" t="s">
         <v>35</v>
       </c>
+      <c r="J1" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="15">
       <c r="B2" s="20" t="s">
@@ -5207,49 +5234,49 @@
     <row r="172" spans="1:9" ht="12.75" customHeight="1">
       <c r="A172" s="7"/>
       <c r="B172" t="s">
-        <v>4</v>
+        <v>444</v>
       </c>
       <c r="D172" t="s">
-        <v>406</v>
+        <v>537</v>
       </c>
       <c r="E172" t="s">
-        <v>65</v>
+        <v>539</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="12.75" customHeight="1">
       <c r="A173" s="7"/>
-      <c r="B173" s="11" t="s">
-        <v>15</v>
+      <c r="B173" t="s">
+        <v>4</v>
+      </c>
+      <c r="D173" t="s">
+        <v>406</v>
+      </c>
+      <c r="E173" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="12.75" customHeight="1">
       <c r="A174" s="7"/>
-      <c r="B174" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E174" t="s">
-        <v>66</v>
+      <c r="B174" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="12.75" customHeight="1">
       <c r="A175" s="7"/>
-      <c r="B175" t="s">
-        <v>4</v>
-      </c>
-      <c r="D175" t="s">
-        <v>67</v>
+      <c r="B175" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E175" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="12.75" customHeight="1">
       <c r="A176" s="7"/>
       <c r="B176" t="s">
-        <v>23</v>
-      </c>
-      <c r="C176" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D176" t="s">
-        <v>417</v>
+        <v>67</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="12.75" customHeight="1">
@@ -5258,79 +5285,79 @@
         <v>23</v>
       </c>
       <c r="C177" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D177" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="12.75" customHeight="1">
       <c r="A178" s="7"/>
       <c r="B178" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="C178" t="s">
+        <v>69</v>
       </c>
       <c r="D178" t="s">
-        <v>407</v>
-      </c>
-      <c r="E178" t="s">
-        <v>70</v>
+        <v>418</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="12.75" customHeight="1">
       <c r="A179" s="7"/>
-      <c r="B179" s="11" t="s">
-        <v>15</v>
+      <c r="B179" t="s">
+        <v>4</v>
+      </c>
+      <c r="D179" t="s">
+        <v>407</v>
+      </c>
+      <c r="E179" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="12.75" customHeight="1">
       <c r="A180" s="7"/>
-      <c r="B180" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E180" t="s">
-        <v>71</v>
+      <c r="B180" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="181" spans="1:8" ht="12.75" customHeight="1">
       <c r="A181" s="7"/>
-      <c r="B181" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D181" t="s">
-        <v>72</v>
+      <c r="B181" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E181" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="12.75" customHeight="1">
       <c r="A182" s="7"/>
-      <c r="B182" t="s">
-        <v>41</v>
-      </c>
-      <c r="C182" t="s">
-        <v>48</v>
+      <c r="B182" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="D182" t="s">
-        <v>419</v>
+        <v>72</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="12.75" customHeight="1">
       <c r="A183" s="7"/>
       <c r="B183" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="C183" t="s">
+        <v>48</v>
       </c>
       <c r="D183" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="12.75" customHeight="1">
       <c r="A184" s="7"/>
       <c r="B184" t="s">
-        <v>42</v>
-      </c>
-      <c r="C184" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D184" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="12.75" customHeight="1">
@@ -5339,22 +5366,22 @@
         <v>42</v>
       </c>
       <c r="C185" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D185" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="12.75" customHeight="1">
       <c r="A186" s="7"/>
       <c r="B186" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="C186" t="s">
+        <v>44</v>
       </c>
       <c r="D186" t="s">
-        <v>408</v>
-      </c>
-      <c r="E186" t="s">
-        <v>73</v>
+        <v>422</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="12.75" customHeight="1">
@@ -5363,32 +5390,44 @@
         <v>4</v>
       </c>
       <c r="D187" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E187" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="12.75" customHeight="1">
       <c r="A188" s="7"/>
-      <c r="B188" s="11" t="s">
-        <v>15</v>
+      <c r="B188" t="s">
+        <v>4</v>
+      </c>
+      <c r="D188" t="s">
+        <v>409</v>
+      </c>
+      <c r="E188" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="12.75" customHeight="1">
       <c r="A189" s="7"/>
-      <c r="B189" s="8" t="s">
+      <c r="B189" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A190" s="7"/>
+      <c r="B190" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C189" s="8"/>
-      <c r="D189" s="8"/>
-      <c r="E189" s="8"/>
-      <c r="F189" s="8"/>
-      <c r="G189" s="8"/>
-      <c r="H189" s="8"/>
-    </row>
-    <row r="192" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B192" s="34" t="s">
+      <c r="C190" s="8"/>
+      <c r="D190" s="8"/>
+      <c r="E190" s="8"/>
+      <c r="F190" s="8"/>
+      <c r="G190" s="8"/>
+      <c r="H190" s="8"/>
+    </row>
+    <row r="193" spans="2:2" ht="12.75" customHeight="1">
+      <c r="B193" s="34" t="s">
         <v>380</v>
       </c>
     </row>
@@ -6694,10 +6733,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6731,271 +6770,271 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>327</v>
+        <v>536</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>329</v>
+        <v>534</v>
       </c>
       <c r="B5" t="s">
-        <v>330</v>
+        <v>535</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>329</v>
+      </c>
+      <c r="B7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A8" t="s">
         <v>331</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="12" customHeight="1">
-      <c r="A8" t="s">
-        <v>333</v>
-      </c>
-      <c r="B8" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="12" customHeight="1">
-      <c r="A9" t="s">
-        <v>335</v>
-      </c>
-      <c r="B9" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B10" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B11" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B12" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
+        <v>339</v>
+      </c>
+      <c r="B13" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="12" customHeight="1">
+      <c r="A14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B14" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="12" customHeight="1">
+      <c r="A15" t="s">
         <v>343</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="42" customHeight="1">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" ht="42" customHeight="1">
+      <c r="A16" t="s">
         <v>345</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>346</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A15" t="s">
-        <v>347</v>
-      </c>
-      <c r="B15" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A16" t="s">
-        <v>349</v>
-      </c>
-      <c r="B16" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B17" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B18" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B19" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B20" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B21" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B22" t="s">
-        <v>362</v>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>359</v>
+      </c>
+      <c r="B23" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" customHeight="1">
       <c r="A24" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A25" t="s">
-        <v>364</v>
-      </c>
-      <c r="B25" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>363</v>
       </c>
       <c r="B26" t="s">
-        <v>366</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="12.75" customHeight="1">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>364</v>
       </c>
       <c r="B27" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="12.75" customHeight="1">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12.75" customHeight="1">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="12.75" customHeight="1">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="12.75" customHeight="1">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="12.75" customHeight="1">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="12.75" customHeight="1">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A37" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="12.75" customHeight="1">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
         <v>123</v>
@@ -7003,9 +7042,25 @@
     </row>
     <row r="42" spans="1:2" ht="12.75" customHeight="1">
       <c r="A42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A44" t="s">
         <v>109</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed back button from main menu
</commit_message>
<xml_diff>
--- a/neonatal/neonatal.xlsx
+++ b/neonatal/neonatal.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="541">
   <si>
     <t>type</t>
   </si>
@@ -431,9 +431,6 @@
   </si>
   <si>
     <t>label back_to_main</t>
-  </si>
-  <si>
-    <t>menu menu</t>
   </si>
   <si>
     <t>menu</t>
@@ -1850,6 +1847,12 @@
   </si>
   <si>
     <t>data('birthW') &amp;&amp; data('currW')&amp;&amp;data('currW')-data('birthW')&gt;=0</t>
+  </si>
+  <si>
+    <t>main_menu</t>
+  </si>
+  <si>
+    <t>main_menu menu</t>
   </si>
 </sst>
 </file>
@@ -3297,8 +3300,8 @@
   <dimension ref="A1:J193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D172" sqref="D172"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3340,7 +3343,7 @@
         <v>35</v>
       </c>
       <c r="J1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15">
@@ -3354,13 +3357,13 @@
     </row>
     <row r="3" spans="1:10" ht="12">
       <c r="B3" s="21" t="s">
+        <v>540</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="19" t="s">
         <v>137</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>138</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="2" t="s">
@@ -3370,12 +3373,12 @@
     <row r="4" spans="1:10" s="33" customFormat="1" ht="15">
       <c r="A4" s="12"/>
       <c r="B4" s="31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
@@ -3386,12 +3389,12 @@
     <row r="5" spans="1:10" ht="12">
       <c r="A5" s="12"/>
       <c r="B5" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -3399,10 +3402,10 @@
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -3414,13 +3417,13 @@
     <row r="7" spans="1:10" ht="12">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>373</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>374</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
@@ -3437,7 +3440,7 @@
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
       <c r="E8" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="12"/>
@@ -3455,7 +3458,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1">
@@ -3464,7 +3467,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E10" s="14"/>
     </row>
@@ -3474,7 +3477,7 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12">
@@ -3497,7 +3500,7 @@
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
       <c r="E13" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3506,7 +3509,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3523,7 +3526,7 @@
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="12" customFormat="1" ht="13" customHeight="1">
@@ -3533,7 +3536,7 @@
       </c>
       <c r="D17"/>
       <c r="I17" s="12" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3545,7 +3548,7 @@
     <row r="19" spans="1:10" ht="15">
       <c r="A19" s="16"/>
       <c r="B19" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="29"/>
@@ -3555,22 +3558,22 @@
     <row r="21" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A21" s="35"/>
       <c r="B21" s="14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="B22" s="14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -3578,10 +3581,10 @@
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -3593,13 +3596,13 @@
     <row r="24" spans="1:10" ht="12">
       <c r="A24" s="12"/>
       <c r="B24" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>430</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
@@ -3610,15 +3613,15 @@
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
       <c r="E25" s="38" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
@@ -3627,12 +3630,12 @@
     <row r="26" spans="1:10" ht="12.75" customHeight="1">
       <c r="A26" s="7"/>
       <c r="B26" s="38" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
       <c r="E26" s="38" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
@@ -3641,7 +3644,7 @@
     <row r="27" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="39"/>
       <c r="B27" s="13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -3653,13 +3656,13 @@
     <row r="28" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="39"/>
       <c r="B28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D28" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E28"/>
       <c r="F28" t="s">
@@ -3669,20 +3672,20 @@
     <row r="29" spans="1:10" ht="24">
       <c r="A29" s="7"/>
       <c r="B29" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>441</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="18" customHeight="1">
@@ -3693,46 +3696,46 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F30" s="2"/>
       <c r="I30" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="18" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>446</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="18" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F32" s="2"/>
       <c r="I32" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15">
       <c r="A33" s="7"/>
       <c r="B33" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -3757,7 +3760,7 @@
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
@@ -3770,7 +3773,7 @@
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
       <c r="E36" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -3856,7 +3859,7 @@
         <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1">
@@ -3865,7 +3868,7 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E44" t="s">
         <v>25</v>
@@ -3896,7 +3899,7 @@
         <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1">
@@ -3905,7 +3908,7 @@
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E48" t="s">
         <v>32</v>
@@ -3950,7 +3953,7 @@
         <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="12.75" customHeight="1">
@@ -3962,7 +3965,7 @@
         <v>64</v>
       </c>
       <c r="D54" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="12.75" customHeight="1">
@@ -3971,7 +3974,7 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E55" t="s">
         <v>65</v>
@@ -4010,7 +4013,7 @@
         <v>68</v>
       </c>
       <c r="D59" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="12.75" customHeight="1">
@@ -4022,7 +4025,7 @@
         <v>69</v>
       </c>
       <c r="D60" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="12.75" customHeight="1">
@@ -4031,7 +4034,7 @@
         <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E61" t="s">
         <v>70</v>
@@ -4066,12 +4069,12 @@
     </row>
     <row r="65" spans="1:8" ht="12.75" customHeight="1">
       <c r="B65" s="14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
       <c r="E65" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F65" s="15"/>
       <c r="G65" s="15"/>
@@ -4079,12 +4082,12 @@
     </row>
     <row r="66" spans="1:8" ht="12.75" customHeight="1">
       <c r="B66" s="14" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
       <c r="E66" s="15" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
@@ -4092,10 +4095,10 @@
     </row>
     <row r="67" spans="1:8" ht="12.75" customHeight="1">
       <c r="A67" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
@@ -4107,13 +4110,13 @@
     <row r="68" spans="1:8" ht="12.75" customHeight="1">
       <c r="A68" s="16"/>
       <c r="B68" t="s">
+        <v>502</v>
+      </c>
+      <c r="C68" t="s">
         <v>503</v>
       </c>
-      <c r="C68" t="s">
-        <v>504</v>
-      </c>
       <c r="D68" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E68" s="40"/>
       <c r="F68" t="s">
@@ -4130,7 +4133,7 @@
       <c r="C69" s="30"/>
       <c r="D69" s="30"/>
       <c r="E69" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F69" s="30"/>
       <c r="G69" s="30"/>
@@ -4143,7 +4146,7 @@
       </c>
       <c r="C70" s="30"/>
       <c r="D70" s="41" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E70" s="30"/>
       <c r="F70" s="30"/>
@@ -4164,7 +4167,7 @@
       <c r="C72" s="30"/>
       <c r="D72" s="30"/>
       <c r="E72" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F72" s="30"/>
       <c r="G72" s="30"/>
@@ -4177,7 +4180,7 @@
       </c>
       <c r="C73" s="30"/>
       <c r="D73" s="41" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E73" s="30"/>
       <c r="F73" s="30"/>
@@ -4193,7 +4196,7 @@
     <row r="75" spans="1:8" ht="12.75" customHeight="1">
       <c r="A75" s="7"/>
       <c r="B75" s="8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
@@ -4213,12 +4216,12 @@
     </row>
     <row r="77" spans="1:8" ht="12.75" customHeight="1">
       <c r="B77" s="14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="15"/>
       <c r="E77" s="15" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
@@ -4226,12 +4229,12 @@
     </row>
     <row r="78" spans="1:8" ht="12.75" customHeight="1">
       <c r="B78" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15"/>
       <c r="E78" s="15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F78" s="15"/>
       <c r="G78" s="15"/>
@@ -4239,10 +4242,10 @@
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1">
       <c r="A79" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -4254,13 +4257,13 @@
     <row r="80" spans="1:8" ht="12.75" customHeight="1">
       <c r="A80" s="16"/>
       <c r="B80" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C80" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D80" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E80" s="40"/>
       <c r="F80" t="s">
@@ -4272,211 +4275,211 @@
     <row r="81" spans="1:8" ht="12">
       <c r="A81" s="7"/>
       <c r="B81" s="43" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C81" s="43" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="11" customHeight="1">
       <c r="A82" s="7"/>
       <c r="B82" t="s">
+        <v>448</v>
+      </c>
+      <c r="C82" t="s">
+        <v>155</v>
+      </c>
+      <c r="D82" t="s">
         <v>449</v>
       </c>
-      <c r="C82" t="s">
-        <v>156</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E82" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="F82" t="s">
         <v>451</v>
-      </c>
-      <c r="F82" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="11" customHeight="1">
       <c r="A83" s="7"/>
       <c r="B83" t="s">
+        <v>452</v>
+      </c>
+      <c r="C83" t="s">
+        <v>166</v>
+      </c>
+      <c r="D83" t="s">
         <v>453</v>
       </c>
-      <c r="C83" t="s">
-        <v>167</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="E83" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>455</v>
-      </c>
       <c r="F83" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="11" customHeight="1">
       <c r="A84" s="7"/>
       <c r="B84" t="s">
+        <v>455</v>
+      </c>
+      <c r="C84" t="s">
+        <v>179</v>
+      </c>
+      <c r="D84" t="s">
         <v>456</v>
       </c>
-      <c r="C84" t="s">
-        <v>180</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="E84" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>458</v>
-      </c>
       <c r="F84" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="11" customHeight="1">
       <c r="A85" s="7"/>
       <c r="B85" t="s">
+        <v>458</v>
+      </c>
+      <c r="C85" t="s">
+        <v>190</v>
+      </c>
+      <c r="D85" t="s">
         <v>459</v>
       </c>
-      <c r="C85" t="s">
-        <v>191</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E85" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>461</v>
-      </c>
       <c r="F85" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="11" customHeight="1">
       <c r="A86" s="7"/>
       <c r="B86" t="s">
+        <v>461</v>
+      </c>
+      <c r="C86" t="s">
+        <v>205</v>
+      </c>
+      <c r="D86" t="s">
         <v>462</v>
       </c>
-      <c r="C86" t="s">
-        <v>206</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E86" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>464</v>
-      </c>
       <c r="F86" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="11" customHeight="1">
       <c r="A87" s="7"/>
       <c r="B87" t="s">
+        <v>464</v>
+      </c>
+      <c r="C87" t="s">
+        <v>218</v>
+      </c>
+      <c r="D87" t="s">
         <v>465</v>
       </c>
-      <c r="C87" t="s">
-        <v>219</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>467</v>
-      </c>
       <c r="F87" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="11" customHeight="1">
       <c r="A88" s="7"/>
       <c r="B88" t="s">
+        <v>467</v>
+      </c>
+      <c r="C88" t="s">
+        <v>231</v>
+      </c>
+      <c r="D88" t="s">
         <v>468</v>
       </c>
-      <c r="C88" t="s">
-        <v>232</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E88" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="11" customHeight="1">
       <c r="A89" s="7"/>
       <c r="B89" t="s">
+        <v>470</v>
+      </c>
+      <c r="C89" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" t="s">
         <v>471</v>
       </c>
-      <c r="C89" t="s">
-        <v>247</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="E89" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="11" customHeight="1">
       <c r="A90" s="7"/>
       <c r="B90" t="s">
+        <v>473</v>
+      </c>
+      <c r="C90" t="s">
+        <v>259</v>
+      </c>
+      <c r="D90" t="s">
         <v>474</v>
       </c>
-      <c r="C90" t="s">
-        <v>260</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E90" s="2" t="s">
         <v>475</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="11" customHeight="1">
       <c r="A91" s="7"/>
       <c r="B91" t="s">
+        <v>476</v>
+      </c>
+      <c r="C91" t="s">
+        <v>274</v>
+      </c>
+      <c r="D91" t="s">
         <v>477</v>
       </c>
-      <c r="C91" t="s">
-        <v>275</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E91" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="11" customHeight="1">
       <c r="A92" s="7"/>
       <c r="B92" t="s">
+        <v>479</v>
+      </c>
+      <c r="C92" t="s">
+        <v>287</v>
+      </c>
+      <c r="D92" t="s">
         <v>480</v>
       </c>
-      <c r="C92" t="s">
-        <v>288</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E92" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="12" customHeight="1">
       <c r="A93" s="7"/>
       <c r="B93" t="s">
+        <v>482</v>
+      </c>
+      <c r="C93" t="s">
+        <v>302</v>
+      </c>
+      <c r="D93" t="s">
         <v>483</v>
       </c>
-      <c r="C93" t="s">
-        <v>303</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="E93" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="12.75" customHeight="1">
@@ -4521,7 +4524,7 @@
         <v>14</v>
       </c>
       <c r="E100" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="24">
@@ -4563,7 +4566,7 @@
         <v>24</v>
       </c>
       <c r="D104" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="12.75" customHeight="1">
@@ -4572,7 +4575,7 @@
         <v>4</v>
       </c>
       <c r="D105" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E105" t="s">
         <v>25</v>
@@ -4603,7 +4606,7 @@
         <v>27</v>
       </c>
       <c r="D108" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="12.75" customHeight="1">
@@ -4612,7 +4615,7 @@
         <v>4</v>
       </c>
       <c r="D109" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E109" t="s">
         <v>32</v>
@@ -4636,7 +4639,7 @@
         <v>14</v>
       </c>
       <c r="E112" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="12.75" customHeight="1">
@@ -4657,7 +4660,7 @@
         <v>48</v>
       </c>
       <c r="D114" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" customHeight="1">
@@ -4666,7 +4669,7 @@
         <v>4</v>
       </c>
       <c r="D115" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="12.75" customHeight="1">
@@ -4678,7 +4681,7 @@
         <v>43</v>
       </c>
       <c r="D116" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="12.75" customHeight="1">
@@ -4690,7 +4693,7 @@
         <v>44</v>
       </c>
       <c r="D117" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="12.75" customHeight="1">
@@ -4699,7 +4702,7 @@
         <v>4</v>
       </c>
       <c r="D118" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E118" t="s">
         <v>73</v>
@@ -4711,7 +4714,7 @@
         <v>4</v>
       </c>
       <c r="D119" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E119" t="s">
         <v>45</v>
@@ -4726,7 +4729,7 @@
     <row r="121" spans="1:10" ht="20" customHeight="1">
       <c r="A121" s="7"/>
       <c r="B121" s="8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C121" s="13"/>
       <c r="D121" s="13"/>
@@ -4738,7 +4741,7 @@
     <row r="122" spans="1:10" ht="15">
       <c r="A122" s="16"/>
       <c r="B122" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C122" s="28"/>
       <c r="D122" s="29"/>
@@ -4748,22 +4751,22 @@
     <row r="124" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A124" s="35"/>
       <c r="B124" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="E124" s="15" t="s">
         <v>392</v>
-      </c>
-      <c r="E124" s="15" t="s">
-        <v>393</v>
       </c>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
     </row>
     <row r="125" spans="1:10" ht="12.75" customHeight="1">
       <c r="B125" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C125" s="15"/>
       <c r="D125" s="15"/>
       <c r="E125" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F125" s="15"/>
       <c r="G125" s="15"/>
@@ -4771,7 +4774,7 @@
     </row>
     <row r="126" spans="1:10" ht="15">
       <c r="A126" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B126" s="8" t="s">
         <v>75</v>
@@ -4838,7 +4841,7 @@
         <v>116</v>
       </c>
       <c r="D132" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="61" customHeight="1">
@@ -4847,7 +4850,7 @@
         <v>4</v>
       </c>
       <c r="D133" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E133" t="s">
         <v>117</v>
@@ -4907,7 +4910,7 @@
         <v>118</v>
       </c>
       <c r="D139" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="75" customHeight="1">
@@ -4916,7 +4919,7 @@
         <v>4</v>
       </c>
       <c r="D140" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E140" t="s">
         <v>119</v>
@@ -4928,7 +4931,7 @@
         <v>4</v>
       </c>
       <c r="D141" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E141" t="s">
         <v>119</v>
@@ -4940,7 +4943,7 @@
         <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E142" t="s">
         <v>119</v>
@@ -4997,7 +5000,7 @@
         <v>4</v>
       </c>
       <c r="D148" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="12.75" customHeight="1">
@@ -5021,30 +5024,30 @@
     <row r="152" spans="1:9" s="14" customFormat="1" ht="15">
       <c r="A152" s="27"/>
       <c r="B152" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C152" s="36"/>
       <c r="D152" s="37"/>
       <c r="E152" s="15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F152" s="36"/>
     </row>
     <row r="153" spans="1:9" s="14" customFormat="1" ht="15">
       <c r="A153" s="27"/>
       <c r="B153" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C153" s="36"/>
       <c r="D153" s="37"/>
       <c r="E153" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F153" s="36"/>
     </row>
     <row r="154" spans="1:9" ht="15">
       <c r="A154" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B154" s="8" t="s">
         <v>54</v>
@@ -5122,7 +5125,7 @@
         <v>24</v>
       </c>
       <c r="D160" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="12.75" customHeight="1">
@@ -5131,7 +5134,7 @@
         <v>4</v>
       </c>
       <c r="D161" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E161" t="s">
         <v>25</v>
@@ -5162,7 +5165,7 @@
         <v>27</v>
       </c>
       <c r="D164" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="12.75" customHeight="1">
@@ -5171,7 +5174,7 @@
         <v>4</v>
       </c>
       <c r="D165" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E165" t="s">
         <v>32</v>
@@ -5216,7 +5219,7 @@
         <v>63</v>
       </c>
       <c r="D170" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="12.75" customHeight="1">
@@ -5228,19 +5231,19 @@
         <v>64</v>
       </c>
       <c r="D171" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="12.75" customHeight="1">
       <c r="A172" s="7"/>
       <c r="B172" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D172" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E172" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="12.75" customHeight="1">
@@ -5249,10 +5252,10 @@
         <v>4</v>
       </c>
       <c r="D173" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E173" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="12.75" customHeight="1">
@@ -5288,7 +5291,7 @@
         <v>68</v>
       </c>
       <c r="D177" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="12.75" customHeight="1">
@@ -5300,7 +5303,7 @@
         <v>69</v>
       </c>
       <c r="D178" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="12.75" customHeight="1">
@@ -5309,7 +5312,7 @@
         <v>4</v>
       </c>
       <c r="D179" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E179" t="s">
         <v>70</v>
@@ -5348,7 +5351,7 @@
         <v>48</v>
       </c>
       <c r="D183" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="12.75" customHeight="1">
@@ -5357,7 +5360,7 @@
         <v>4</v>
       </c>
       <c r="D184" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="12.75" customHeight="1">
@@ -5369,7 +5372,7 @@
         <v>43</v>
       </c>
       <c r="D185" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="12.75" customHeight="1">
@@ -5381,7 +5384,7 @@
         <v>44</v>
       </c>
       <c r="D186" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="12.75" customHeight="1">
@@ -5390,7 +5393,7 @@
         <v>4</v>
       </c>
       <c r="D187" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E187" t="s">
         <v>73</v>
@@ -5402,7 +5405,7 @@
         <v>4</v>
       </c>
       <c r="D188" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E188" t="s">
         <v>45</v>
@@ -5428,7 +5431,7 @@
     </row>
     <row r="193" spans="2:2" ht="12.75" customHeight="1">
       <c r="B193" s="34" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -5468,98 +5471,98 @@
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1">
       <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" t="s">
         <v>144</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>145</v>
-      </c>
-      <c r="C7" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" t="s">
         <v>147</v>
-      </c>
-      <c r="C8" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C9" t="s">
         <v>389</v>
-      </c>
-      <c r="C9" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1">
       <c r="A12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -5567,68 +5570,68 @@
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" t="s">
+        <v>429</v>
+      </c>
+      <c r="B13" t="s">
         <v>430</v>
       </c>
-      <c r="B13" t="s">
-        <v>431</v>
-      </c>
       <c r="C13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
       <c r="A16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" t="s">
         <v>149</v>
       </c>
-      <c r="B16" t="s">
-        <v>150</v>
-      </c>
       <c r="C16" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" t="s">
         <v>154</v>
-      </c>
-      <c r="C19" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1">
@@ -5787,40 +5790,40 @@
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
+        <v>503</v>
+      </c>
+      <c r="B39" t="s">
         <v>504</v>
       </c>
-      <c r="B39" t="s">
-        <v>505</v>
-      </c>
       <c r="C39" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B40" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C40" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
+        <v>518</v>
+      </c>
+      <c r="B42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" t="s">
         <v>519</v>
-      </c>
-      <c r="B42" t="s">
-        <v>153</v>
-      </c>
-      <c r="C42" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B43" t="s">
         <v>91</v>
@@ -5831,7 +5834,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
@@ -5842,882 +5845,882 @@
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" t="s">
         <v>156</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>157</v>
-      </c>
-      <c r="D46" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B47" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" t="s">
         <v>159</v>
-      </c>
-      <c r="D47" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B48" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" t="s">
         <v>161</v>
-      </c>
-      <c r="D48" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" t="s">
         <v>163</v>
-      </c>
-      <c r="D49" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B50" t="s">
+        <v>164</v>
+      </c>
+      <c r="D50" t="s">
         <v>165</v>
-      </c>
-      <c r="D50" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
+        <v>166</v>
+      </c>
+      <c r="B52" t="s">
         <v>167</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>168</v>
-      </c>
-      <c r="D52" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B53" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" t="s">
         <v>170</v>
-      </c>
-      <c r="D53" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B54" t="s">
+        <v>171</v>
+      </c>
+      <c r="D54" t="s">
         <v>172</v>
-      </c>
-      <c r="D54" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B55" t="s">
+        <v>173</v>
+      </c>
+      <c r="D55" t="s">
         <v>174</v>
-      </c>
-      <c r="D55" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B56" t="s">
+        <v>175</v>
+      </c>
+      <c r="D56" t="s">
         <v>176</v>
-      </c>
-      <c r="D56" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B57" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" t="s">
         <v>178</v>
-      </c>
-      <c r="D57" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" t="s">
         <v>180</v>
-      </c>
-      <c r="B59" t="s">
-        <v>181</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B60" t="s">
+        <v>182</v>
+      </c>
+      <c r="D60" t="s">
         <v>183</v>
-      </c>
-      <c r="D60" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B61" t="s">
+        <v>184</v>
+      </c>
+      <c r="D61" t="s">
         <v>185</v>
-      </c>
-      <c r="D61" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B62" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" t="s">
         <v>187</v>
-      </c>
-      <c r="D62" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B63" t="s">
+        <v>188</v>
+      </c>
+      <c r="D63" t="s">
         <v>189</v>
-      </c>
-      <c r="D63" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
       <c r="A65" t="s">
+        <v>190</v>
+      </c>
+      <c r="B65" t="s">
         <v>191</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
         <v>192</v>
-      </c>
-      <c r="D65" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B66" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B67" t="s">
+        <v>195</v>
+      </c>
+      <c r="D67" t="s">
         <v>196</v>
-      </c>
-      <c r="D67" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B68" t="s">
+        <v>197</v>
+      </c>
+      <c r="D68" t="s">
         <v>198</v>
-      </c>
-      <c r="D68" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B69" t="s">
+        <v>199</v>
+      </c>
+      <c r="D69" t="s">
         <v>200</v>
-      </c>
-      <c r="D69" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B70" t="s">
+        <v>201</v>
+      </c>
+      <c r="D70" t="s">
         <v>202</v>
-      </c>
-      <c r="D70" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B71" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" t="s">
         <v>204</v>
-      </c>
-      <c r="D71" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
+        <v>205</v>
+      </c>
+      <c r="B73" t="s">
         <v>206</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>207</v>
-      </c>
-      <c r="D73" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B75" t="s">
+        <v>210</v>
+      </c>
+      <c r="D75" t="s">
         <v>211</v>
-      </c>
-      <c r="D75" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B76" t="s">
+        <v>212</v>
+      </c>
+      <c r="D76" t="s">
         <v>213</v>
-      </c>
-      <c r="D76" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B77" t="s">
+        <v>214</v>
+      </c>
+      <c r="D77" t="s">
         <v>215</v>
-      </c>
-      <c r="D77" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B78" t="s">
+        <v>216</v>
+      </c>
+      <c r="D78" t="s">
         <v>217</v>
-      </c>
-      <c r="D78" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
       <c r="A80" t="s">
+        <v>218</v>
+      </c>
+      <c r="B80" t="s">
         <v>219</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>220</v>
-      </c>
-      <c r="D80" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B81" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B82" t="s">
+        <v>223</v>
+      </c>
+      <c r="D82" t="s">
         <v>224</v>
-      </c>
-      <c r="D82" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="12.75" customHeight="1">
       <c r="A83" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D83" t="s">
         <v>226</v>
-      </c>
-      <c r="D83" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B84" t="s">
+        <v>227</v>
+      </c>
+      <c r="D84" t="s">
         <v>228</v>
-      </c>
-      <c r="D84" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
       <c r="A85" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B85" t="s">
+        <v>229</v>
+      </c>
+      <c r="D85" t="s">
         <v>230</v>
-      </c>
-      <c r="D85" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75" customHeight="1">
       <c r="A87" t="s">
+        <v>231</v>
+      </c>
+      <c r="B87" t="s">
         <v>232</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>233</v>
-      </c>
-      <c r="C87" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
       <c r="A88" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B88" t="s">
+        <v>234</v>
+      </c>
+      <c r="C88" t="s">
         <v>235</v>
-      </c>
-      <c r="C88" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B89" t="s">
+        <v>236</v>
+      </c>
+      <c r="C89" t="s">
         <v>237</v>
-      </c>
-      <c r="C89" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="12.75" customHeight="1">
       <c r="A90" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B90" t="s">
+        <v>238</v>
+      </c>
+      <c r="C90" t="s">
         <v>239</v>
-      </c>
-      <c r="C90" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B91" t="s">
+        <v>240</v>
+      </c>
+      <c r="C91" t="s">
         <v>241</v>
-      </c>
-      <c r="C91" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B92" t="s">
+        <v>242</v>
+      </c>
+      <c r="C92" t="s">
         <v>243</v>
-      </c>
-      <c r="C92" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="12.75" customHeight="1">
       <c r="A93" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B93" t="s">
+        <v>244</v>
+      </c>
+      <c r="C93" t="s">
         <v>245</v>
-      </c>
-      <c r="C93" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
+        <v>246</v>
+      </c>
+      <c r="B95" t="s">
         <v>247</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>248</v>
-      </c>
-      <c r="C95" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B96" t="s">
+        <v>249</v>
+      </c>
+      <c r="C96" t="s">
         <v>250</v>
-      </c>
-      <c r="C96" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B97" t="s">
+        <v>251</v>
+      </c>
+      <c r="C97" t="s">
         <v>252</v>
-      </c>
-      <c r="C97" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1">
       <c r="A98" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B98" t="s">
+        <v>253</v>
+      </c>
+      <c r="C98" t="s">
         <v>254</v>
-      </c>
-      <c r="C98" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B99" t="s">
+        <v>255</v>
+      </c>
+      <c r="C99" t="s">
         <v>256</v>
-      </c>
-      <c r="C99" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B100" t="s">
+        <v>257</v>
+      </c>
+      <c r="C100" t="s">
         <v>258</v>
-      </c>
-      <c r="C100" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
+        <v>259</v>
+      </c>
+      <c r="B102" t="s">
         <v>260</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>261</v>
-      </c>
-      <c r="C102" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B103" t="s">
+        <v>262</v>
+      </c>
+      <c r="C103" t="s">
         <v>263</v>
-      </c>
-      <c r="C103" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B104" t="s">
+        <v>264</v>
+      </c>
+      <c r="C104" t="s">
         <v>265</v>
-      </c>
-      <c r="C104" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1">
       <c r="A105" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B105" t="s">
+        <v>266</v>
+      </c>
+      <c r="C105" t="s">
         <v>267</v>
-      </c>
-      <c r="C105" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B106" t="s">
+        <v>268</v>
+      </c>
+      <c r="C106" t="s">
         <v>269</v>
-      </c>
-      <c r="C106" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B107" t="s">
+        <v>270</v>
+      </c>
+      <c r="C107" t="s">
         <v>271</v>
-      </c>
-      <c r="C107" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
       <c r="A108" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B108" t="s">
+        <v>272</v>
+      </c>
+      <c r="C108" t="s">
         <v>273</v>
-      </c>
-      <c r="C108" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
+        <v>274</v>
+      </c>
+      <c r="B110" t="s">
         <v>275</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>276</v>
-      </c>
-      <c r="C110" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B111" t="s">
+        <v>277</v>
+      </c>
+      <c r="C111" t="s">
         <v>278</v>
-      </c>
-      <c r="C111" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B112" t="s">
+        <v>279</v>
+      </c>
+      <c r="C112" t="s">
         <v>280</v>
-      </c>
-      <c r="C112" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="12.75" customHeight="1">
       <c r="A113" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B113" t="s">
+        <v>281</v>
+      </c>
+      <c r="C113" t="s">
         <v>282</v>
-      </c>
-      <c r="C113" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B114" t="s">
+        <v>283</v>
+      </c>
+      <c r="C114" t="s">
         <v>284</v>
-      </c>
-      <c r="C114" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B115" t="s">
+        <v>285</v>
+      </c>
+      <c r="C115" t="s">
         <v>286</v>
-      </c>
-      <c r="C115" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1">
       <c r="A117" t="s">
+        <v>287</v>
+      </c>
+      <c r="B117" t="s">
         <v>288</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>289</v>
-      </c>
-      <c r="C117" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B118" t="s">
+        <v>290</v>
+      </c>
+      <c r="C118" t="s">
         <v>291</v>
-      </c>
-      <c r="C118" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B119" t="s">
+        <v>292</v>
+      </c>
+      <c r="C119" t="s">
         <v>293</v>
-      </c>
-      <c r="C119" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="12.75" customHeight="1">
       <c r="A120" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B120" t="s">
+        <v>294</v>
+      </c>
+      <c r="C120" t="s">
         <v>295</v>
-      </c>
-      <c r="C120" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B121" t="s">
+        <v>296</v>
+      </c>
+      <c r="C121" t="s">
         <v>297</v>
-      </c>
-      <c r="C121" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B122" t="s">
+        <v>298</v>
+      </c>
+      <c r="C122" t="s">
         <v>299</v>
-      </c>
-      <c r="C122" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="12.75" customHeight="1">
       <c r="A123" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B123" t="s">
+        <v>300</v>
+      </c>
+      <c r="C123" t="s">
         <v>301</v>
-      </c>
-      <c r="C123" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
+        <v>302</v>
+      </c>
+      <c r="B125" t="s">
         <v>303</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>304</v>
-      </c>
-      <c r="C125" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B126" t="s">
+        <v>305</v>
+      </c>
+      <c r="C126" t="s">
         <v>306</v>
-      </c>
-      <c r="C126" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B127" t="s">
+        <v>307</v>
+      </c>
+      <c r="C127" t="s">
         <v>308</v>
-      </c>
-      <c r="C127" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="12.75" customHeight="1">
       <c r="A128" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B128" t="s">
+        <v>309</v>
+      </c>
+      <c r="C128" t="s">
         <v>310</v>
-      </c>
-      <c r="C128" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="12.75" customHeight="1">
       <c r="A129" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B129" t="s">
+        <v>311</v>
+      </c>
+      <c r="C129" t="s">
         <v>312</v>
-      </c>
-      <c r="C129" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="12.75" customHeight="1">
       <c r="A130" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B130" t="s">
+        <v>313</v>
+      </c>
+      <c r="C130" t="s">
         <v>314</v>
-      </c>
-      <c r="C130" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="12.75" customHeight="1">
       <c r="A132" t="s">
+        <v>315</v>
+      </c>
+      <c r="B132" t="s">
         <v>316</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>317</v>
-      </c>
-      <c r="C132" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="12.75" customHeight="1">
       <c r="A133" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B133" t="s">
+        <v>318</v>
+      </c>
+      <c r="C133" t="s">
         <v>319</v>
-      </c>
-      <c r="C133" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="12.75" customHeight="1">
       <c r="A135" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D135" t="s">
         <v>321</v>
-      </c>
-      <c r="D135" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="12.75" customHeight="1">
       <c r="A136" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D136" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="12.75" customHeight="1">
       <c r="A137" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D137" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="12.75" customHeight="1">
       <c r="A138" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D138" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="12.75" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D139" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -6770,167 +6773,167 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
+        <v>533</v>
+      </c>
+      <c r="B5" t="s">
         <v>534</v>
-      </c>
-      <c r="B5" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B6" t="s">
         <v>327</v>
-      </c>
-      <c r="B6" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="1">
       <c r="A7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B7" t="s">
         <v>329</v>
-      </c>
-      <c r="B7" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12.75" customHeight="1">
       <c r="A8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B8" t="s">
         <v>331</v>
-      </c>
-      <c r="B8" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" t="s">
         <v>333</v>
-      </c>
-      <c r="B10" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
+        <v>334</v>
+      </c>
+      <c r="B11" t="s">
         <v>335</v>
-      </c>
-      <c r="B11" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B12" t="s">
         <v>337</v>
-      </c>
-      <c r="B12" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
+        <v>338</v>
+      </c>
+      <c r="B13" t="s">
         <v>339</v>
-      </c>
-      <c r="B13" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1">
       <c r="A14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B14" t="s">
         <v>341</v>
-      </c>
-      <c r="B14" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12" customHeight="1">
       <c r="A15" t="s">
+        <v>342</v>
+      </c>
+      <c r="B15" t="s">
         <v>343</v>
-      </c>
-      <c r="B15" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="42" customHeight="1">
       <c r="A16" t="s">
+        <v>344</v>
+      </c>
+      <c r="B16" t="s">
         <v>345</v>
-      </c>
-      <c r="B16" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
+        <v>346</v>
+      </c>
+      <c r="B17" t="s">
         <v>347</v>
-      </c>
-      <c r="B17" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
+        <v>348</v>
+      </c>
+      <c r="B18" t="s">
         <v>349</v>
-      </c>
-      <c r="B18" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
+        <v>350</v>
+      </c>
+      <c r="B19" t="s">
         <v>351</v>
-      </c>
-      <c r="B19" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
+        <v>352</v>
+      </c>
+      <c r="B20" t="s">
         <v>353</v>
-      </c>
-      <c r="B20" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" t="s">
+        <v>354</v>
+      </c>
+      <c r="B21" t="s">
         <v>355</v>
-      </c>
-      <c r="B21" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
+        <v>356</v>
+      </c>
+      <c r="B22" t="s">
         <v>357</v>
-      </c>
-      <c r="B22" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12.75" customHeight="1">
       <c r="A23" t="s">
+        <v>358</v>
+      </c>
+      <c r="B23" t="s">
         <v>359</v>
-      </c>
-      <c r="B23" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" customHeight="1">
       <c r="A24" t="s">
+        <v>360</v>
+      </c>
+      <c r="B24" t="s">
         <v>361</v>
-      </c>
-      <c r="B24" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -6938,10 +6941,10 @@
     </row>
     <row r="27" spans="1:2" ht="12.75" customHeight="1">
       <c r="A27" t="s">
+        <v>363</v>
+      </c>
+      <c r="B27" t="s">
         <v>364</v>
-      </c>
-      <c r="B27" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="12.75" customHeight="1">
@@ -6949,7 +6952,7 @@
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12.75" customHeight="1">
@@ -6957,7 +6960,7 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="12.75" customHeight="1">
@@ -7098,7 +7101,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
@@ -7106,7 +7109,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
@@ -7114,7 +7117,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -7129,10 +7132,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -7142,31 +7145,39 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B2" t="s">
         <v>385</v>
-      </c>
-      <c r="B2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B4" t="s">
-        <v>386</v>
+        <v>385</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>539</v>
+      </c>
+      <c r="B5" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make sure not negative input for weight lost calculator
</commit_message>
<xml_diff>
--- a/neonatal/neonatal.xlsx
+++ b/neonatal/neonatal.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="543">
   <si>
     <t>type</t>
   </si>
@@ -1831,9 +1831,6 @@
     <t>constraint</t>
   </si>
   <si>
-    <t>data('birthW') &amp;&amp; data('currW')&amp;&amp;data('currW')-data('birthW')&lt;0</t>
-  </si>
-  <si>
     <t>weightGain</t>
   </si>
   <si>
@@ -1849,7 +1846,19 @@
     <t>(calculates.weightGain()*100.0/data('birthW')).toFixed(2)</t>
   </si>
   <si>
-    <t>data('birthW') &amp;&amp; data('currW')&amp;&amp;data('currW')-data('birthW')&gt;=0</t>
+    <t>data('currW')&gt;=0 &amp;&amp; data('birthW') &gt;=0</t>
+  </si>
+  <si>
+    <t>data('birthW') &amp;&amp; data('currW')&amp;&amp;data('currW')-data('birthW')&gt;=0&amp;&amp;data('currW')&gt;=0&amp;&amp;data('birthW')&gt;=0</t>
+  </si>
+  <si>
+    <t>data('birthW') &amp;&amp; data('currW')&amp;&amp;data('currW')-data('birthW')&lt;0&amp;&amp;data('currW')&gt;=0&amp;&amp;data('birthW')&gt;=0</t>
+  </si>
+  <si>
+    <t>data('birthW') &lt; 0 || data('currW') &lt;0</t>
+  </si>
+  <si>
+    <t>Please enter a non-negative number for weight.</t>
   </si>
 </sst>
 </file>
@@ -2017,7 +2026,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="422">
+  <cellStyleXfs count="424">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2362,6 +2371,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2543,7 +2554,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="422">
+  <cellStyles count="424">
     <cellStyle name="20% - Accent4" xfId="343" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2754,6 +2765,7 @@
     <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="243" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2964,6 +2976,7 @@
     <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="244" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3294,10 +3307,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J193"/>
+  <dimension ref="A1:J194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
@@ -5125,7 +5138,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="12.75" customHeight="1">
+    <row r="161" spans="1:10" ht="12.75" customHeight="1">
       <c r="A161" s="7"/>
       <c r="B161" t="s">
         <v>4</v>
@@ -5138,13 +5151,13 @@
       </c>
       <c r="I161" s="9"/>
     </row>
-    <row r="162" spans="1:9" ht="12.75" customHeight="1">
+    <row r="162" spans="1:10" ht="12.75" customHeight="1">
       <c r="A162" s="7"/>
       <c r="B162" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="12.75" customHeight="1">
+    <row r="163" spans="1:10" ht="12.75" customHeight="1">
       <c r="A163" s="7"/>
       <c r="B163" s="10" t="s">
         <v>14</v>
@@ -5153,7 +5166,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="12.75" customHeight="1">
+    <row r="164" spans="1:10" ht="12.75" customHeight="1">
       <c r="A164" s="7"/>
       <c r="B164" t="s">
         <v>23</v>
@@ -5165,7 +5178,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="12.75" customHeight="1">
+    <row r="165" spans="1:10" ht="12.75" customHeight="1">
       <c r="A165" s="7"/>
       <c r="B165" t="s">
         <v>4</v>
@@ -5177,19 +5190,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="12.75" customHeight="1">
+    <row r="166" spans="1:10" ht="12.75" customHeight="1">
       <c r="A166" s="7"/>
       <c r="B166" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="12.75" customHeight="1">
+    <row r="167" spans="1:10" ht="12.75" customHeight="1">
       <c r="A167" s="7"/>
       <c r="B167" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="12.75" customHeight="1">
+    <row r="168" spans="1:10" ht="12.75" customHeight="1">
       <c r="A168" s="7"/>
       <c r="B168" s="10" t="s">
         <v>14</v>
@@ -5198,7 +5211,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="12.75" customHeight="1">
+    <row r="169" spans="1:10" ht="12.75" customHeight="1">
       <c r="A169" s="7"/>
       <c r="B169" t="s">
         <v>4</v>
@@ -5207,7 +5220,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="12.75" customHeight="1">
+    <row r="170" spans="1:10" ht="12.75" customHeight="1">
       <c r="A170" s="7"/>
       <c r="B170" t="s">
         <v>23</v>
@@ -5219,7 +5232,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="12.75" customHeight="1">
+    <row r="171" spans="1:10" ht="12.75" customHeight="1">
       <c r="A171" s="7"/>
       <c r="B171" t="s">
         <v>23</v>
@@ -5231,64 +5244,70 @@
         <v>416</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="12.75" customHeight="1">
+    <row r="172" spans="1:10" ht="12.75" customHeight="1">
       <c r="A172" s="7"/>
       <c r="B172" t="s">
-        <v>444</v>
+        <v>4</v>
       </c>
       <c r="D172" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="E172" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" ht="12.75" customHeight="1">
+        <v>541</v>
+      </c>
+      <c r="J172" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" ht="12.75" customHeight="1">
       <c r="A173" s="7"/>
       <c r="B173" t="s">
+        <v>444</v>
+      </c>
+      <c r="D173" t="s">
+        <v>536</v>
+      </c>
+      <c r="E173" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A174" s="7"/>
+      <c r="B174" t="s">
         <v>4</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D174" t="s">
         <v>406</v>
       </c>
-      <c r="E173" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A174" s="7"/>
-      <c r="B174" s="11" t="s">
+      <c r="E174" t="s">
+        <v>540</v>
+      </c>
+      <c r="J174" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A175" s="7"/>
+      <c r="B175" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A175" s="7"/>
-      <c r="B175" s="10" t="s">
+    <row r="176" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A176" s="7"/>
+      <c r="B176" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E175" t="s">
+      <c r="E176" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A176" s="7"/>
-      <c r="B176" t="s">
-        <v>4</v>
-      </c>
-      <c r="D176" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="12.75" customHeight="1">
       <c r="A177" s="7"/>
       <c r="B177" t="s">
-        <v>23</v>
-      </c>
-      <c r="C177" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D177" t="s">
-        <v>417</v>
+        <v>67</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="12.75" customHeight="1">
@@ -5297,79 +5316,79 @@
         <v>23</v>
       </c>
       <c r="C178" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D178" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="12.75" customHeight="1">
       <c r="A179" s="7"/>
       <c r="B179" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="C179" t="s">
+        <v>69</v>
       </c>
       <c r="D179" t="s">
-        <v>407</v>
-      </c>
-      <c r="E179" t="s">
-        <v>70</v>
+        <v>418</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="12.75" customHeight="1">
       <c r="A180" s="7"/>
-      <c r="B180" s="11" t="s">
-        <v>15</v>
+      <c r="B180" t="s">
+        <v>4</v>
+      </c>
+      <c r="D180" t="s">
+        <v>407</v>
+      </c>
+      <c r="E180" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="181" spans="1:8" ht="12.75" customHeight="1">
       <c r="A181" s="7"/>
-      <c r="B181" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E181" t="s">
-        <v>71</v>
+      <c r="B181" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="12.75" customHeight="1">
       <c r="A182" s="7"/>
-      <c r="B182" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D182" t="s">
-        <v>72</v>
+      <c r="B182" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E182" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="12.75" customHeight="1">
       <c r="A183" s="7"/>
-      <c r="B183" t="s">
-        <v>41</v>
-      </c>
-      <c r="C183" t="s">
-        <v>48</v>
+      <c r="B183" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="D183" t="s">
-        <v>419</v>
+        <v>72</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="12.75" customHeight="1">
       <c r="A184" s="7"/>
       <c r="B184" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="C184" t="s">
+        <v>48</v>
       </c>
       <c r="D184" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="12.75" customHeight="1">
       <c r="A185" s="7"/>
       <c r="B185" t="s">
-        <v>42</v>
-      </c>
-      <c r="C185" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D185" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="12.75" customHeight="1">
@@ -5378,22 +5397,22 @@
         <v>42</v>
       </c>
       <c r="C186" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D186" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="12.75" customHeight="1">
       <c r="A187" s="7"/>
       <c r="B187" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="C187" t="s">
+        <v>44</v>
       </c>
       <c r="D187" t="s">
-        <v>408</v>
-      </c>
-      <c r="E187" t="s">
-        <v>73</v>
+        <v>422</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="12.75" customHeight="1">
@@ -5402,32 +5421,44 @@
         <v>4</v>
       </c>
       <c r="D188" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E188" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="12.75" customHeight="1">
       <c r="A189" s="7"/>
-      <c r="B189" s="11" t="s">
-        <v>15</v>
+      <c r="B189" t="s">
+        <v>4</v>
+      </c>
+      <c r="D189" t="s">
+        <v>409</v>
+      </c>
+      <c r="E189" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="190" spans="1:8" ht="12.75" customHeight="1">
       <c r="A190" s="7"/>
-      <c r="B190" s="8" t="s">
+      <c r="B190" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A191" s="7"/>
+      <c r="B191" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C190" s="8"/>
-      <c r="D190" s="8"/>
-      <c r="E190" s="8"/>
-      <c r="F190" s="8"/>
-      <c r="G190" s="8"/>
-      <c r="H190" s="8"/>
-    </row>
-    <row r="193" spans="2:2" ht="12.75" customHeight="1">
-      <c r="B193" s="34" t="s">
+      <c r="C191" s="8"/>
+      <c r="D191" s="8"/>
+      <c r="E191" s="8"/>
+      <c r="F191" s="8"/>
+      <c r="G191" s="8"/>
+      <c r="H191" s="8"/>
+    </row>
+    <row r="194" spans="2:2" ht="12.75" customHeight="1">
+      <c r="B194" s="34" t="s">
         <v>380</v>
       </c>
     </row>
@@ -6736,7 +6767,7 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6770,18 +6801,18 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
+        <v>533</v>
+      </c>
+      <c r="B5" t="s">
         <v>534</v>
-      </c>
-      <c r="B5" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">

</xml_diff>

<commit_message>
Fixed negative fore medications
</commit_message>
<xml_diff>
--- a/neonatal/neonatal.xlsx
+++ b/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="547">
   <si>
     <t>type</t>
   </si>
@@ -376,13 +376,7 @@
     <t>weightKiloCaffeine</t>
   </si>
   <si>
-    <t>data('weightKiloCaffeine')</t>
-  </si>
-  <si>
     <t>weightKiloChlorothiazide</t>
-  </si>
-  <si>
-    <t>data('weightKiloChlorothiazide')</t>
   </si>
   <si>
     <t>data('weightKiloChlorothiazide')*20</t>
@@ -1862,6 +1856,21 @@
   </si>
   <si>
     <t>main_menu</t>
+  </si>
+  <si>
+    <t>Please enter a positive weight.</t>
+  </si>
+  <si>
+    <t>data('weightKiloChlorothiazide') &amp;&amp; (data('weightKiloChlorothiazide') &gt; 0)</t>
+  </si>
+  <si>
+    <t>data('weightKiloChlorothiazide') &lt;= 0</t>
+  </si>
+  <si>
+    <t>data('weightKiloCaffeine') &lt;= 0</t>
+  </si>
+  <si>
+    <t>data('weightKiloCaffeine') &amp;&amp; (data('weightKiloCaffeine') &gt; 0)</t>
   </si>
 </sst>
 </file>
@@ -2029,7 +2038,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="426">
+  <cellStyleXfs count="430">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2374,6 +2383,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2559,7 +2572,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="426">
+  <cellStyles count="430">
     <cellStyle name="20% - Accent4" xfId="343" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2772,6 +2785,8 @@
     <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="243" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2984,6 +2999,8 @@
     <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="426" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="428" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="244" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3314,11 +3331,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J194"/>
+  <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3333,7 +3350,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="12">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3351,21 +3368,21 @@
         <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I1" t="s">
         <v>35</v>
       </c>
       <c r="J1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15">
       <c r="B2" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="21"/>
@@ -3374,13 +3391,13 @@
     </row>
     <row r="3" spans="1:10" ht="12">
       <c r="B3" s="21" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="2" t="s">
@@ -3390,12 +3407,12 @@
     <row r="4" spans="1:10" s="33" customFormat="1" ht="15">
       <c r="A4" s="12"/>
       <c r="B4" s="31" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
@@ -3406,12 +3423,12 @@
     <row r="5" spans="1:10" ht="12">
       <c r="A5" s="12"/>
       <c r="B5" s="22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -3419,10 +3436,10 @@
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -3434,13 +3451,13 @@
     <row r="7" spans="1:10" ht="12">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
@@ -3457,7 +3474,7 @@
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
       <c r="E8" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="12"/>
@@ -3475,7 +3492,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1">
@@ -3484,7 +3501,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E10" s="14"/>
     </row>
@@ -3494,7 +3511,7 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12">
@@ -3517,7 +3534,7 @@
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
       <c r="E13" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3526,7 +3543,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3543,7 +3560,7 @@
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="12" customFormat="1" ht="13" customHeight="1">
@@ -3553,7 +3570,7 @@
       </c>
       <c r="D17"/>
       <c r="I17" s="12" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3565,7 +3582,7 @@
     <row r="19" spans="1:10" ht="15">
       <c r="A19" s="16"/>
       <c r="B19" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="29"/>
@@ -3575,22 +3592,22 @@
     <row r="21" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A21" s="35"/>
       <c r="B21" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="B22" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -3598,10 +3615,10 @@
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -3613,13 +3630,13 @@
     <row r="24" spans="1:10" ht="12">
       <c r="A24" s="12"/>
       <c r="B24" s="3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
@@ -3630,15 +3647,15 @@
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
       <c r="E25" s="38" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
@@ -3647,12 +3664,12 @@
     <row r="26" spans="1:10" ht="12.75" customHeight="1">
       <c r="A26" s="7"/>
       <c r="B26" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
       <c r="E26" s="38" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
@@ -3661,7 +3678,7 @@
     <row r="27" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="39"/>
       <c r="B27" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -3673,13 +3690,13 @@
     <row r="28" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="39"/>
       <c r="B28" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D28" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E28"/>
       <c r="F28" t="s">
@@ -3689,20 +3706,20 @@
     <row r="29" spans="1:10" ht="24">
       <c r="A29" s="7"/>
       <c r="B29" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="18" customHeight="1">
@@ -3713,46 +3730,46 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F30" s="2"/>
       <c r="I30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="18" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="18" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F32" s="2"/>
       <c r="I32" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15">
       <c r="A33" s="7"/>
       <c r="B33" s="8" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -3777,7 +3794,7 @@
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
@@ -3790,7 +3807,7 @@
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
       <c r="E36" s="15" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -3876,7 +3893,7 @@
         <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1">
@@ -3885,7 +3902,7 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E44" t="s">
         <v>25</v>
@@ -3916,7 +3933,7 @@
         <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1">
@@ -3925,7 +3942,7 @@
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E48" t="s">
         <v>32</v>
@@ -3970,7 +3987,7 @@
         <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="12.75" customHeight="1">
@@ -3982,7 +3999,7 @@
         <v>64</v>
       </c>
       <c r="D54" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="12.75" customHeight="1">
@@ -3991,7 +4008,7 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E55" t="s">
         <v>65</v>
@@ -4030,7 +4047,7 @@
         <v>68</v>
       </c>
       <c r="D59" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="12.75" customHeight="1">
@@ -4042,7 +4059,7 @@
         <v>69</v>
       </c>
       <c r="D60" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="12.75" customHeight="1">
@@ -4051,7 +4068,7 @@
         <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E61" t="s">
         <v>70</v>
@@ -4086,12 +4103,12 @@
     </row>
     <row r="65" spans="1:8" ht="12.75" customHeight="1">
       <c r="B65" s="14" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
       <c r="E65" s="15" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F65" s="15"/>
       <c r="G65" s="15"/>
@@ -4099,12 +4116,12 @@
     </row>
     <row r="66" spans="1:8" ht="12.75" customHeight="1">
       <c r="B66" s="14" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
       <c r="E66" s="15" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
@@ -4112,10 +4129,10 @@
     </row>
     <row r="67" spans="1:8" ht="12.75" customHeight="1">
       <c r="A67" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
@@ -4127,13 +4144,13 @@
     <row r="68" spans="1:8" ht="12.75" customHeight="1">
       <c r="A68" s="16"/>
       <c r="B68" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C68" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D68" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E68" s="40"/>
       <c r="F68" t="s">
@@ -4150,7 +4167,7 @@
       <c r="C69" s="30"/>
       <c r="D69" s="30"/>
       <c r="E69" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F69" s="30"/>
       <c r="G69" s="30"/>
@@ -4163,7 +4180,7 @@
       </c>
       <c r="C70" s="30"/>
       <c r="D70" s="41" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E70" s="30"/>
       <c r="F70" s="30"/>
@@ -4184,7 +4201,7 @@
       <c r="C72" s="30"/>
       <c r="D72" s="30"/>
       <c r="E72" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F72" s="30"/>
       <c r="G72" s="30"/>
@@ -4197,7 +4214,7 @@
       </c>
       <c r="C73" s="30"/>
       <c r="D73" s="41" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E73" s="30"/>
       <c r="F73" s="30"/>
@@ -4213,7 +4230,7 @@
     <row r="75" spans="1:8" ht="12.75" customHeight="1">
       <c r="A75" s="7"/>
       <c r="B75" s="8" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
@@ -4233,12 +4250,12 @@
     </row>
     <row r="77" spans="1:8" ht="12.75" customHeight="1">
       <c r="B77" s="14" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="15"/>
       <c r="E77" s="15" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
@@ -4246,12 +4263,12 @@
     </row>
     <row r="78" spans="1:8" ht="12.75" customHeight="1">
       <c r="B78" s="14" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15"/>
       <c r="E78" s="15" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F78" s="15"/>
       <c r="G78" s="15"/>
@@ -4259,10 +4276,10 @@
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1">
       <c r="A79" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -4274,13 +4291,13 @@
     <row r="80" spans="1:8" ht="12.75" customHeight="1">
       <c r="A80" s="16"/>
       <c r="B80" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C80" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D80" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E80" s="40"/>
       <c r="F80" t="s">
@@ -4292,211 +4309,211 @@
     <row r="81" spans="1:8" ht="12">
       <c r="A81" s="7"/>
       <c r="B81" s="43" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C81" s="43" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="11" customHeight="1">
       <c r="A82" s="7"/>
       <c r="B82" t="s">
+        <v>446</v>
+      </c>
+      <c r="C82" t="s">
+        <v>153</v>
+      </c>
+      <c r="D82" t="s">
+        <v>447</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="C82" t="s">
-        <v>155</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="F82" t="s">
         <v>449</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="F82" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="11" customHeight="1">
       <c r="A83" s="7"/>
       <c r="B83" t="s">
+        <v>450</v>
+      </c>
+      <c r="C83" t="s">
+        <v>164</v>
+      </c>
+      <c r="D83" t="s">
+        <v>451</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="C83" t="s">
-        <v>166</v>
-      </c>
-      <c r="D83" t="s">
-        <v>453</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>454</v>
-      </c>
       <c r="F83" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="11" customHeight="1">
       <c r="A84" s="7"/>
       <c r="B84" t="s">
+        <v>453</v>
+      </c>
+      <c r="C84" t="s">
+        <v>177</v>
+      </c>
+      <c r="D84" t="s">
+        <v>454</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="C84" t="s">
-        <v>179</v>
-      </c>
-      <c r="D84" t="s">
-        <v>456</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>457</v>
-      </c>
       <c r="F84" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="11" customHeight="1">
       <c r="A85" s="7"/>
       <c r="B85" t="s">
+        <v>456</v>
+      </c>
+      <c r="C85" t="s">
+        <v>188</v>
+      </c>
+      <c r="D85" t="s">
+        <v>457</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="C85" t="s">
-        <v>190</v>
-      </c>
-      <c r="D85" t="s">
-        <v>459</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>460</v>
-      </c>
       <c r="F85" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="11" customHeight="1">
       <c r="A86" s="7"/>
       <c r="B86" t="s">
+        <v>459</v>
+      </c>
+      <c r="C86" t="s">
+        <v>203</v>
+      </c>
+      <c r="D86" t="s">
+        <v>460</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="C86" t="s">
-        <v>205</v>
-      </c>
-      <c r="D86" t="s">
-        <v>462</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>463</v>
-      </c>
       <c r="F86" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="11" customHeight="1">
       <c r="A87" s="7"/>
       <c r="B87" t="s">
+        <v>462</v>
+      </c>
+      <c r="C87" t="s">
+        <v>216</v>
+      </c>
+      <c r="D87" t="s">
+        <v>463</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C87" t="s">
-        <v>218</v>
-      </c>
-      <c r="D87" t="s">
-        <v>465</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>466</v>
-      </c>
       <c r="F87" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="11" customHeight="1">
       <c r="A88" s="7"/>
       <c r="B88" t="s">
+        <v>465</v>
+      </c>
+      <c r="C88" t="s">
+        <v>229</v>
+      </c>
+      <c r="D88" t="s">
+        <v>466</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="C88" t="s">
-        <v>231</v>
-      </c>
-      <c r="D88" t="s">
-        <v>468</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="11" customHeight="1">
       <c r="A89" s="7"/>
       <c r="B89" t="s">
+        <v>468</v>
+      </c>
+      <c r="C89" t="s">
+        <v>244</v>
+      </c>
+      <c r="D89" t="s">
+        <v>469</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="C89" t="s">
-        <v>246</v>
-      </c>
-      <c r="D89" t="s">
-        <v>471</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="11" customHeight="1">
       <c r="A90" s="7"/>
       <c r="B90" t="s">
+        <v>471</v>
+      </c>
+      <c r="C90" t="s">
+        <v>257</v>
+      </c>
+      <c r="D90" t="s">
+        <v>472</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="C90" t="s">
-        <v>259</v>
-      </c>
-      <c r="D90" t="s">
-        <v>474</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="11" customHeight="1">
       <c r="A91" s="7"/>
       <c r="B91" t="s">
+        <v>474</v>
+      </c>
+      <c r="C91" t="s">
+        <v>272</v>
+      </c>
+      <c r="D91" t="s">
+        <v>475</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="C91" t="s">
-        <v>274</v>
-      </c>
-      <c r="D91" t="s">
-        <v>477</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="11" customHeight="1">
       <c r="A92" s="7"/>
       <c r="B92" t="s">
+        <v>477</v>
+      </c>
+      <c r="C92" t="s">
+        <v>285</v>
+      </c>
+      <c r="D92" t="s">
+        <v>478</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>479</v>
-      </c>
-      <c r="C92" t="s">
-        <v>287</v>
-      </c>
-      <c r="D92" t="s">
-        <v>480</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="12" customHeight="1">
       <c r="A93" s="7"/>
       <c r="B93" t="s">
+        <v>480</v>
+      </c>
+      <c r="C93" t="s">
+        <v>300</v>
+      </c>
+      <c r="D93" t="s">
+        <v>481</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="C93" t="s">
-        <v>302</v>
-      </c>
-      <c r="D93" t="s">
-        <v>483</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="12.75" customHeight="1">
@@ -4541,7 +4558,7 @@
         <v>14</v>
       </c>
       <c r="E100" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="24">
@@ -4583,7 +4600,7 @@
         <v>24</v>
       </c>
       <c r="D104" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="12.75" customHeight="1">
@@ -4592,7 +4609,7 @@
         <v>4</v>
       </c>
       <c r="D105" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E105" t="s">
         <v>25</v>
@@ -4623,7 +4640,7 @@
         <v>27</v>
       </c>
       <c r="D108" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="12.75" customHeight="1">
@@ -4632,7 +4649,7 @@
         <v>4</v>
       </c>
       <c r="D109" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E109" t="s">
         <v>32</v>
@@ -4656,7 +4673,7 @@
         <v>14</v>
       </c>
       <c r="E112" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="12.75" customHeight="1">
@@ -4677,7 +4694,7 @@
         <v>48</v>
       </c>
       <c r="D114" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" customHeight="1">
@@ -4686,7 +4703,7 @@
         <v>4</v>
       </c>
       <c r="D115" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="12.75" customHeight="1">
@@ -4698,7 +4715,7 @@
         <v>43</v>
       </c>
       <c r="D116" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="12.75" customHeight="1">
@@ -4710,7 +4727,7 @@
         <v>44</v>
       </c>
       <c r="D117" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="12.75" customHeight="1">
@@ -4719,7 +4736,7 @@
         <v>4</v>
       </c>
       <c r="D118" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E118" t="s">
         <v>73</v>
@@ -4731,7 +4748,7 @@
         <v>4</v>
       </c>
       <c r="D119" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E119" t="s">
         <v>45</v>
@@ -4746,7 +4763,7 @@
     <row r="121" spans="1:10" ht="20" customHeight="1">
       <c r="A121" s="7"/>
       <c r="B121" s="8" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C121" s="13"/>
       <c r="D121" s="13"/>
@@ -4758,7 +4775,7 @@
     <row r="122" spans="1:10" ht="15">
       <c r="A122" s="16"/>
       <c r="B122" s="8" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C122" s="28"/>
       <c r="D122" s="29"/>
@@ -4768,22 +4785,22 @@
     <row r="124" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A124" s="35"/>
       <c r="B124" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E124" s="15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
     </row>
     <row r="125" spans="1:10" ht="12.75" customHeight="1">
       <c r="B125" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C125" s="15"/>
       <c r="D125" s="15"/>
       <c r="E125" s="15" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F125" s="15"/>
       <c r="G125" s="15"/>
@@ -4791,7 +4808,7 @@
     </row>
     <row r="126" spans="1:10" ht="15">
       <c r="A126" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B126" s="8" t="s">
         <v>75</v>
@@ -4858,157 +4875,163 @@
         <v>116</v>
       </c>
       <c r="D132" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="61" customHeight="1">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="12.75" customHeight="1">
       <c r="A133" s="7"/>
       <c r="B133" t="s">
         <v>4</v>
       </c>
       <c r="D133" t="s">
-        <v>395</v>
+        <v>542</v>
       </c>
       <c r="E133" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="12.75" customHeight="1">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="61" customHeight="1">
       <c r="A134" s="7"/>
       <c r="B134" t="s">
         <v>4</v>
       </c>
-      <c r="C134" t="s">
-        <v>34</v>
-      </c>
-      <c r="I134" t="s">
-        <v>36</v>
+      <c r="D134" t="s">
+        <v>393</v>
+      </c>
+      <c r="E134" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="12.75" customHeight="1">
       <c r="A135" s="7"/>
-      <c r="B135" s="6" t="s">
-        <v>15</v>
+      <c r="B135" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135" t="s">
+        <v>34</v>
+      </c>
+      <c r="I135" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="12.75" customHeight="1">
       <c r="A136" s="7"/>
-      <c r="B136" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E136" t="s">
-        <v>105</v>
+      <c r="B136" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="12.75" customHeight="1">
       <c r="A137" s="7"/>
-      <c r="B137" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D137" t="s">
-        <v>115</v>
+      <c r="B137" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E137" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="12.75" customHeight="1">
       <c r="A138" s="7"/>
-      <c r="B138" t="s">
+      <c r="B138" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D138" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="12.75" customHeight="1">
       <c r="A139" s="7"/>
       <c r="B139" t="s">
-        <v>23</v>
-      </c>
-      <c r="C139" t="s">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="D139" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="75" customHeight="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="12.75" customHeight="1">
       <c r="A140" s="7"/>
       <c r="B140" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="C140" t="s">
+        <v>117</v>
       </c>
       <c r="D140" t="s">
-        <v>396</v>
-      </c>
-      <c r="E140" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" ht="36" customHeight="1">
-      <c r="A141" s="7"/>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A141" s="16"/>
       <c r="B141" t="s">
         <v>4</v>
       </c>
       <c r="D141" t="s">
-        <v>397</v>
+        <v>542</v>
       </c>
       <c r="E141" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" ht="41" customHeight="1">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="75" customHeight="1">
       <c r="A142" s="7"/>
       <c r="B142" t="s">
         <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E142" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="12" customHeight="1">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="36" customHeight="1">
       <c r="A143" s="7"/>
       <c r="B143" t="s">
         <v>4</v>
       </c>
-      <c r="C143" t="s">
+      <c r="D143" t="s">
+        <v>395</v>
+      </c>
+      <c r="E143" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="41" customHeight="1">
+      <c r="A144" s="7"/>
+      <c r="B144" t="s">
+        <v>4</v>
+      </c>
+      <c r="D144" t="s">
+        <v>396</v>
+      </c>
+      <c r="E144" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="12" customHeight="1">
+      <c r="A145" s="7"/>
+      <c r="B145" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" t="s">
         <v>103</v>
       </c>
-      <c r="I143" t="s">
+      <c r="I145" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A144" s="7"/>
-      <c r="B144" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A145" s="7"/>
-      <c r="B145" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E145" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="12.75" customHeight="1">
       <c r="A146" s="7"/>
-      <c r="B146" t="s">
-        <v>4</v>
-      </c>
-      <c r="C146" t="s">
-        <v>129</v>
-      </c>
-      <c r="I146" t="s">
-        <v>130</v>
+      <c r="B146" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="12.75" customHeight="1">
       <c r="A147" s="7"/>
-      <c r="B147" s="6" t="s">
-        <v>15</v>
+      <c r="B147" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E147" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="12.75" customHeight="1">
@@ -5016,8 +5039,11 @@
       <c r="B148" t="s">
         <v>4</v>
       </c>
-      <c r="D148" t="s">
-        <v>409</v>
+      <c r="C148" t="s">
+        <v>127</v>
+      </c>
+      <c r="I148" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="12.75" customHeight="1">
@@ -5028,254 +5054,242 @@
     </row>
     <row r="150" spans="1:9" ht="12.75" customHeight="1">
       <c r="A150" s="7"/>
-      <c r="B150" s="8" t="s">
+      <c r="B150" t="s">
+        <v>4</v>
+      </c>
+      <c r="D150" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A151" s="7"/>
+      <c r="B151" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A152" s="7"/>
+      <c r="B152" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C150" s="13"/>
-      <c r="D150" s="13"/>
-      <c r="E150" s="13"/>
-      <c r="F150" s="13"/>
-      <c r="G150" s="13"/>
-      <c r="H150" s="13"/>
-    </row>
-    <row r="152" spans="1:9" s="14" customFormat="1" ht="15">
-      <c r="A152" s="27"/>
-      <c r="B152" s="14" t="s">
+      <c r="C152" s="13"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
+      <c r="F152" s="13"/>
+      <c r="G152" s="13"/>
+      <c r="H152" s="13"/>
+    </row>
+    <row r="154" spans="1:9" s="14" customFormat="1" ht="15">
+      <c r="A154" s="27"/>
+      <c r="B154" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="C154" s="36"/>
+      <c r="D154" s="37"/>
+      <c r="E154" s="15" t="s">
+        <v>398</v>
+      </c>
+      <c r="F154" s="36"/>
+    </row>
+    <row r="155" spans="1:9" s="14" customFormat="1" ht="15">
+      <c r="A155" s="27"/>
+      <c r="B155" s="14" t="s">
         <v>399</v>
       </c>
-      <c r="C152" s="36"/>
-      <c r="D152" s="37"/>
-      <c r="E152" s="15" t="s">
+      <c r="C155" s="36"/>
+      <c r="D155" s="37"/>
+      <c r="E155" s="15" t="s">
         <v>400</v>
       </c>
-      <c r="F152" s="36"/>
-    </row>
-    <row r="153" spans="1:9" s="14" customFormat="1" ht="15">
-      <c r="A153" s="27"/>
-      <c r="B153" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="C153" s="36"/>
-      <c r="D153" s="37"/>
-      <c r="E153" s="15" t="s">
-        <v>402</v>
-      </c>
-      <c r="F153" s="36"/>
-    </row>
-    <row r="154" spans="1:9" ht="15">
-      <c r="A154" s="7" t="s">
-        <v>494</v>
-      </c>
-      <c r="B154" s="8" t="s">
+      <c r="F155" s="36"/>
+    </row>
+    <row r="156" spans="1:9" ht="15">
+      <c r="A156" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="B156" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
-      <c r="E154" s="8"/>
-      <c r="F154" s="8"/>
-      <c r="G154" s="8"/>
-      <c r="H154" s="8"/>
-    </row>
-    <row r="155" spans="1:9" ht="15">
-      <c r="A155" s="7"/>
-      <c r="B155" t="s">
-        <v>55</v>
-      </c>
-      <c r="C155" t="s">
-        <v>56</v>
-      </c>
-      <c r="D155" t="s">
-        <v>57</v>
-      </c>
-      <c r="E155" s="30"/>
-      <c r="F155" t="s">
-        <v>58</v>
-      </c>
-      <c r="G155" s="9"/>
-      <c r="H155" s="9"/>
-    </row>
-    <row r="156" spans="1:9" ht="12">
-      <c r="A156" s="7"/>
-      <c r="B156" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E156" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" ht="24">
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
+      <c r="F156" s="8"/>
+      <c r="G156" s="8"/>
+      <c r="H156" s="8"/>
+    </row>
+    <row r="157" spans="1:9" ht="15">
       <c r="A157" s="7"/>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>55</v>
+      </c>
+      <c r="C157" t="s">
+        <v>56</v>
       </c>
       <c r="D157" t="s">
-        <v>60</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E157" s="30"/>
+      <c r="F157" t="s">
+        <v>58</v>
+      </c>
+      <c r="G157" s="9"/>
+      <c r="H157" s="9"/>
     </row>
     <row r="158" spans="1:9" ht="12">
       <c r="A158" s="7"/>
-      <c r="B158" t="s">
-        <v>21</v>
-      </c>
-      <c r="C158" t="s">
-        <v>16</v>
-      </c>
-      <c r="F158" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" ht="12">
+      <c r="B158" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E158" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="24">
       <c r="A159" s="7"/>
-      <c r="B159" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E159" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" ht="24">
+      <c r="B159" t="s">
+        <v>4</v>
+      </c>
+      <c r="D159" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="12">
       <c r="A160" s="7"/>
       <c r="B160" t="s">
+        <v>21</v>
+      </c>
+      <c r="C160" t="s">
+        <v>16</v>
+      </c>
+      <c r="F160" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" ht="12">
+      <c r="A161" s="7"/>
+      <c r="B161" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E161" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" ht="24">
+      <c r="A162" s="7"/>
+      <c r="B162" t="s">
         <v>23</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C162" t="s">
         <v>24</v>
       </c>
-      <c r="D160" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A161" s="7"/>
-      <c r="B161" t="s">
-        <v>4</v>
-      </c>
-      <c r="D161" t="s">
-        <v>403</v>
-      </c>
-      <c r="E161" t="s">
-        <v>25</v>
-      </c>
-      <c r="I161" s="9"/>
-    </row>
-    <row r="162" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A162" s="7"/>
-      <c r="B162" s="11" t="s">
-        <v>15</v>
+      <c r="D162" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="163" spans="1:10" ht="12.75" customHeight="1">
       <c r="A163" s="7"/>
-      <c r="B163" s="10" t="s">
-        <v>14</v>
+      <c r="B163" t="s">
+        <v>4</v>
+      </c>
+      <c r="D163" t="s">
+        <v>401</v>
       </c>
       <c r="E163" t="s">
-        <v>26</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I163" s="9"/>
     </row>
     <row r="164" spans="1:10" ht="12.75" customHeight="1">
       <c r="A164" s="7"/>
-      <c r="B164" t="s">
-        <v>23</v>
-      </c>
-      <c r="C164" t="s">
-        <v>27</v>
-      </c>
-      <c r="D164" t="s">
-        <v>413</v>
+      <c r="B164" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="165" spans="1:10" ht="12.75" customHeight="1">
       <c r="A165" s="7"/>
-      <c r="B165" t="s">
-        <v>4</v>
-      </c>
-      <c r="D165" t="s">
-        <v>404</v>
+      <c r="B165" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E165" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="166" spans="1:10" ht="12.75" customHeight="1">
       <c r="A166" s="7"/>
-      <c r="B166" s="11" t="s">
-        <v>15</v>
+      <c r="B166" t="s">
+        <v>23</v>
+      </c>
+      <c r="C166" t="s">
+        <v>27</v>
+      </c>
+      <c r="D166" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="167" spans="1:10" ht="12.75" customHeight="1">
       <c r="A167" s="7"/>
-      <c r="B167" s="11" t="s">
-        <v>15</v>
+      <c r="B167" t="s">
+        <v>4</v>
+      </c>
+      <c r="D167" t="s">
+        <v>402</v>
+      </c>
+      <c r="E167" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="168" spans="1:10" ht="12.75" customHeight="1">
       <c r="A168" s="7"/>
-      <c r="B168" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E168" t="s">
-        <v>61</v>
+      <c r="B168" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="169" spans="1:10" ht="12.75" customHeight="1">
       <c r="A169" s="7"/>
-      <c r="B169" t="s">
-        <v>4</v>
-      </c>
-      <c r="D169" t="s">
-        <v>62</v>
+      <c r="B169" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="170" spans="1:10" ht="12.75" customHeight="1">
       <c r="A170" s="7"/>
-      <c r="B170" t="s">
-        <v>23</v>
-      </c>
-      <c r="C170" t="s">
-        <v>63</v>
-      </c>
-      <c r="D170" t="s">
-        <v>414</v>
+      <c r="B170" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E170" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="171" spans="1:10" ht="12.75" customHeight="1">
       <c r="A171" s="7"/>
       <c r="B171" t="s">
-        <v>23</v>
-      </c>
-      <c r="C171" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="D171" t="s">
-        <v>415</v>
+        <v>62</v>
       </c>
     </row>
     <row r="172" spans="1:10" ht="12.75" customHeight="1">
       <c r="A172" s="7"/>
       <c r="B172" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="C172" t="s">
+        <v>63</v>
       </c>
       <c r="D172" t="s">
-        <v>541</v>
-      </c>
-      <c r="E172" t="s">
-        <v>540</v>
-      </c>
-      <c r="J172" t="s">
-        <v>537</v>
+        <v>412</v>
       </c>
     </row>
     <row r="173" spans="1:10" ht="12.75" customHeight="1">
       <c r="A173" s="7"/>
       <c r="B173" t="s">
-        <v>443</v>
+        <v>23</v>
+      </c>
+      <c r="C173" t="s">
+        <v>64</v>
       </c>
       <c r="D173" t="s">
-        <v>535</v>
-      </c>
-      <c r="E173" t="s">
-        <v>538</v>
+        <v>413</v>
       </c>
     </row>
     <row r="174" spans="1:10" ht="12.75" customHeight="1">
@@ -5284,189 +5298,216 @@
         <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>405</v>
+        <v>539</v>
       </c>
       <c r="E174" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J174" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="175" spans="1:10" ht="12.75" customHeight="1">
       <c r="A175" s="7"/>
-      <c r="B175" s="11" t="s">
-        <v>15</v>
+      <c r="B175" t="s">
+        <v>441</v>
+      </c>
+      <c r="D175" t="s">
+        <v>533</v>
+      </c>
+      <c r="E175" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="176" spans="1:10" ht="12.75" customHeight="1">
       <c r="A176" s="7"/>
-      <c r="B176" s="10" t="s">
+      <c r="B176" t="s">
+        <v>4</v>
+      </c>
+      <c r="D176" t="s">
+        <v>403</v>
+      </c>
+      <c r="E176" t="s">
+        <v>537</v>
+      </c>
+      <c r="J176" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A177" s="7"/>
+      <c r="B177" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A178" s="7"/>
+      <c r="B178" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E178" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A177" s="7"/>
-      <c r="B177" t="s">
-        <v>4</v>
-      </c>
-      <c r="D177" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A178" s="7"/>
-      <c r="B178" t="s">
-        <v>23</v>
-      </c>
-      <c r="C178" t="s">
-        <v>68</v>
-      </c>
-      <c r="D178" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" ht="12.75" customHeight="1">
+    <row r="179" spans="1:5" ht="12.75" customHeight="1">
       <c r="A179" s="7"/>
       <c r="B179" t="s">
-        <v>23</v>
-      </c>
-      <c r="C179" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="D179" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" ht="12.75" customHeight="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="12.75" customHeight="1">
       <c r="A180" s="7"/>
       <c r="B180" t="s">
+        <v>23</v>
+      </c>
+      <c r="C180" t="s">
+        <v>68</v>
+      </c>
+      <c r="D180" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A181" s="7"/>
+      <c r="B181" t="s">
+        <v>23</v>
+      </c>
+      <c r="C181" t="s">
+        <v>69</v>
+      </c>
+      <c r="D181" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A182" s="7"/>
+      <c r="B182" t="s">
         <v>4</v>
       </c>
-      <c r="D180" t="s">
-        <v>406</v>
-      </c>
-      <c r="E180" t="s">
+      <c r="D182" t="s">
+        <v>404</v>
+      </c>
+      <c r="E182" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A181" s="7"/>
-      <c r="B181" s="11" t="s">
+    <row r="183" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A183" s="7"/>
+      <c r="B183" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A182" s="7"/>
-      <c r="B182" s="10" t="s">
+    <row r="184" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A184" s="7"/>
+      <c r="B184" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E184" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A183" s="7"/>
-      <c r="B183" s="12" t="s">
+    <row r="185" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A185" s="7"/>
+      <c r="B185" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D185" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A184" s="7"/>
-      <c r="B184" t="s">
-        <v>41</v>
-      </c>
-      <c r="C184" t="s">
-        <v>48</v>
-      </c>
-      <c r="D184" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A185" s="7"/>
-      <c r="B185" t="s">
-        <v>4</v>
-      </c>
-      <c r="D185" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" ht="12.75" customHeight="1">
+    <row r="186" spans="1:5" ht="12.75" customHeight="1">
       <c r="A186" s="7"/>
       <c r="B186" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C186" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D186" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" ht="12.75" customHeight="1">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="12.75" customHeight="1">
       <c r="A187" s="7"/>
       <c r="B187" t="s">
-        <v>42</v>
-      </c>
-      <c r="C187" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D187" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" ht="12.75" customHeight="1">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" ht="12.75" customHeight="1">
       <c r="A188" s="7"/>
       <c r="B188" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="C188" t="s">
+        <v>43</v>
       </c>
       <c r="D188" t="s">
-        <v>407</v>
-      </c>
-      <c r="E188" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" ht="12.75" customHeight="1">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="12.75" customHeight="1">
       <c r="A189" s="7"/>
       <c r="B189" t="s">
+        <v>42</v>
+      </c>
+      <c r="C189" t="s">
+        <v>44</v>
+      </c>
+      <c r="D189" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A190" s="7"/>
+      <c r="B190" t="s">
         <v>4</v>
       </c>
-      <c r="D189" t="s">
-        <v>408</v>
-      </c>
-      <c r="E189" t="s">
+      <c r="D190" t="s">
+        <v>405</v>
+      </c>
+      <c r="E190" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A191" s="7"/>
+      <c r="B191" t="s">
+        <v>4</v>
+      </c>
+      <c r="D191" t="s">
+        <v>406</v>
+      </c>
+      <c r="E191" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A190" s="7"/>
-      <c r="B190" s="11" t="s">
+    <row r="192" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A192" s="7"/>
+      <c r="B192" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A191" s="7"/>
-      <c r="B191" s="8" t="s">
+    <row r="193" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A193" s="7"/>
+      <c r="B193" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C191" s="8"/>
-      <c r="D191" s="8"/>
-      <c r="E191" s="8"/>
-      <c r="F191" s="8"/>
-      <c r="G191" s="8"/>
-      <c r="H191" s="8"/>
-    </row>
-    <row r="194" spans="2:2" ht="12.75" customHeight="1">
-      <c r="B194" s="34" t="s">
-        <v>379</v>
+      <c r="C193" s="8"/>
+      <c r="D193" s="8"/>
+      <c r="E193" s="8"/>
+      <c r="F193" s="8"/>
+      <c r="G193" s="8"/>
+      <c r="H193" s="8"/>
+    </row>
+    <row r="196" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B196" s="34" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -5501,103 +5542,103 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D3" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1">
       <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
         <v>143</v>
-      </c>
-      <c r="B7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C7" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1">
       <c r="A12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -5605,68 +5646,68 @@
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" t="s">
+        <v>427</v>
+      </c>
+      <c r="B14" t="s">
         <v>429</v>
       </c>
-      <c r="B14" t="s">
-        <v>431</v>
-      </c>
       <c r="C14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" t="s">
         <v>148</v>
       </c>
-      <c r="B17" t="s">
-        <v>150</v>
-      </c>
       <c r="C17" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C18" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1">
@@ -5784,10 +5825,10 @@
         <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.75" customHeight="1">
@@ -5825,40 +5866,40 @@
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B39" t="s">
+        <v>502</v>
+      </c>
+      <c r="C39" t="s">
         <v>504</v>
-      </c>
-      <c r="C39" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
+        <v>501</v>
+      </c>
+      <c r="B40" t="s">
         <v>503</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>505</v>
-      </c>
-      <c r="C40" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C42" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B43" t="s">
         <v>91</v>
@@ -5869,7 +5910,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
@@ -5880,882 +5921,882 @@
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" t="s">
         <v>155</v>
-      </c>
-      <c r="B46" t="s">
-        <v>156</v>
-      </c>
-      <c r="D46" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B48" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D48" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B49" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D49" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B50" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D50" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" t="s">
         <v>166</v>
-      </c>
-      <c r="B52" t="s">
-        <v>167</v>
-      </c>
-      <c r="D52" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B53" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D53" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B55" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D55" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D56" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D57" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B59" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B60" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D60" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B61" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D61" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D62" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
       <c r="A65" t="s">
+        <v>188</v>
+      </c>
+      <c r="B65" t="s">
+        <v>189</v>
+      </c>
+      <c r="D65" t="s">
         <v>190</v>
-      </c>
-      <c r="B65" t="s">
-        <v>191</v>
-      </c>
-      <c r="D65" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B66" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D67" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B68" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D69" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B70" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D70" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B71" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D71" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
+        <v>203</v>
+      </c>
+      <c r="B73" t="s">
+        <v>204</v>
+      </c>
+      <c r="D73" t="s">
         <v>205</v>
-      </c>
-      <c r="B73" t="s">
-        <v>206</v>
-      </c>
-      <c r="D73" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B74" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B75" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D75" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B76" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D76" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B77" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D77" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B78" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D78" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
       <c r="A80" t="s">
+        <v>216</v>
+      </c>
+      <c r="B80" t="s">
+        <v>217</v>
+      </c>
+      <c r="D80" t="s">
         <v>218</v>
-      </c>
-      <c r="B80" t="s">
-        <v>219</v>
-      </c>
-      <c r="D80" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B81" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B82" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D82" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="12.75" customHeight="1">
       <c r="A83" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B83" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D83" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B84" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D84" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
       <c r="A85" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B85" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D85" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75" customHeight="1">
       <c r="A87" t="s">
+        <v>229</v>
+      </c>
+      <c r="B87" t="s">
+        <v>230</v>
+      </c>
+      <c r="C87" t="s">
         <v>231</v>
-      </c>
-      <c r="B87" t="s">
-        <v>232</v>
-      </c>
-      <c r="C87" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
       <c r="A88" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B88" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C88" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B89" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C89" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="12.75" customHeight="1">
       <c r="A90" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B90" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C90" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B91" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C91" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B92" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C92" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="12.75" customHeight="1">
       <c r="A93" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B93" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C93" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
+        <v>244</v>
+      </c>
+      <c r="B95" t="s">
+        <v>245</v>
+      </c>
+      <c r="C95" t="s">
         <v>246</v>
-      </c>
-      <c r="B95" t="s">
-        <v>247</v>
-      </c>
-      <c r="C95" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B96" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C96" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B97" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C97" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1">
       <c r="A98" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B98" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C98" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B99" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C99" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B100" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C100" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
+        <v>257</v>
+      </c>
+      <c r="B102" t="s">
+        <v>258</v>
+      </c>
+      <c r="C102" t="s">
         <v>259</v>
-      </c>
-      <c r="B102" t="s">
-        <v>260</v>
-      </c>
-      <c r="C102" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B103" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C103" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B104" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C104" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1">
       <c r="A105" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B105" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C105" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B106" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C106" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B107" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C107" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
       <c r="A108" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B108" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C108" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
+        <v>272</v>
+      </c>
+      <c r="B110" t="s">
+        <v>273</v>
+      </c>
+      <c r="C110" t="s">
         <v>274</v>
-      </c>
-      <c r="B110" t="s">
-        <v>275</v>
-      </c>
-      <c r="C110" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B111" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C111" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B112" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C112" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="12.75" customHeight="1">
       <c r="A113" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B113" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C113" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B114" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C114" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B115" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C115" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1">
       <c r="A117" t="s">
+        <v>285</v>
+      </c>
+      <c r="B117" t="s">
+        <v>286</v>
+      </c>
+      <c r="C117" t="s">
         <v>287</v>
-      </c>
-      <c r="B117" t="s">
-        <v>288</v>
-      </c>
-      <c r="C117" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B118" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C118" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B119" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C119" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="12.75" customHeight="1">
       <c r="A120" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B120" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C120" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B121" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C121" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B122" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C122" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="12.75" customHeight="1">
       <c r="A123" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B123" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C123" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
+        <v>300</v>
+      </c>
+      <c r="B125" t="s">
+        <v>301</v>
+      </c>
+      <c r="C125" t="s">
         <v>302</v>
-      </c>
-      <c r="B125" t="s">
-        <v>303</v>
-      </c>
-      <c r="C125" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B126" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C126" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B127" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C127" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="12.75" customHeight="1">
       <c r="A128" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B128" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C128" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="12.75" customHeight="1">
       <c r="A129" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B129" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C129" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="12.75" customHeight="1">
       <c r="A130" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B130" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C130" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="12.75" customHeight="1">
       <c r="A132" t="s">
+        <v>313</v>
+      </c>
+      <c r="B132" t="s">
+        <v>314</v>
+      </c>
+      <c r="C132" t="s">
         <v>315</v>
-      </c>
-      <c r="B132" t="s">
-        <v>316</v>
-      </c>
-      <c r="C132" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="12.75" customHeight="1">
       <c r="A133" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B133" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C133" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="12.75" customHeight="1">
       <c r="A135" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D135" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="12.75" customHeight="1">
       <c r="A136" t="s">
+        <v>318</v>
+      </c>
+      <c r="D136" t="s">
         <v>320</v>
-      </c>
-      <c r="D136" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="12.75" customHeight="1">
       <c r="A137" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D137" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="12.75" customHeight="1">
       <c r="A138" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D138" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="12.75" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D139" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -6808,167 +6849,167 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
+        <v>532</v>
+      </c>
+      <c r="B4" t="s">
         <v>534</v>
-      </c>
-      <c r="B4" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="1">
       <c r="A7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12.75" customHeight="1">
       <c r="A8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1">
       <c r="A14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12" customHeight="1">
       <c r="A15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="42" customHeight="1">
       <c r="A16" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B17" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B18" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B20" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B21" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B22" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12.75" customHeight="1">
       <c r="A23" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B23" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" customHeight="1">
       <c r="A24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B24" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -6976,10 +7017,10 @@
     </row>
     <row r="27" spans="1:2" ht="12.75" customHeight="1">
       <c r="A27" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B27" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="12.75" customHeight="1">
@@ -6987,7 +7028,7 @@
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12.75" customHeight="1">
@@ -6995,7 +7036,7 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="12.75" customHeight="1">
@@ -7019,7 +7060,7 @@
         <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="12.75" customHeight="1">
@@ -7027,7 +7068,7 @@
         <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="12.75" customHeight="1">
@@ -7035,7 +7076,7 @@
         <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="12.75" customHeight="1">
@@ -7043,7 +7084,7 @@
         <v>102</v>
       </c>
       <c r="B36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="12.75" customHeight="1">
@@ -7051,7 +7092,7 @@
         <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="12.75" customHeight="1">
@@ -7059,7 +7100,7 @@
         <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="12.75" customHeight="1">
@@ -7067,7 +7108,7 @@
         <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="12.75" customHeight="1">
@@ -7075,7 +7116,7 @@
         <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="12.75" customHeight="1">
@@ -7083,7 +7124,7 @@
         <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="12.75" customHeight="1">
@@ -7091,7 +7132,7 @@
         <v>112</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="12.75" customHeight="1">
@@ -7099,7 +7140,7 @@
         <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -7136,7 +7177,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
@@ -7144,7 +7185,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
@@ -7152,7 +7193,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -7169,8 +7210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -7180,39 +7221,39 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed negatives in more calculotrs
</commit_message>
<xml_diff>
--- a/neonatal/neonatal.xlsx
+++ b/neonatal/neonatal.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="555">
   <si>
     <t>type</t>
   </si>
@@ -1871,6 +1871,30 @@
   </si>
   <si>
     <t>data('weightKiloCaffeine') &amp;&amp; (data('weightKiloCaffeine') &gt; 0)</t>
+  </si>
+  <si>
+    <t>Please enter positive weight.</t>
+  </si>
+  <si>
+    <t>data('weightKilo') &lt;= 0</t>
+  </si>
+  <si>
+    <t>data('weightKilo') &gt; 0</t>
+  </si>
+  <si>
+    <t>data('weightPound') &lt;= 0</t>
+  </si>
+  <si>
+    <t>data('weightPound') &gt; 0</t>
+  </si>
+  <si>
+    <t>Please enter positive values for Total Fluids and Dextros Percentage.</t>
+  </si>
+  <si>
+    <t>data('totalFluid') &lt;= 0 || data('dextrosePerc') &lt;= 0</t>
+  </si>
+  <si>
+    <t>data('totalFluid') &gt; 0 &amp;&amp; data('dextrosePerc') &gt; 0</t>
   </si>
 </sst>
 </file>
@@ -2038,7 +2062,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="430">
+  <cellStyleXfs count="436">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2383,6 +2407,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2572,7 +2602,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="430">
+  <cellStyles count="436">
     <cellStyle name="20% - Accent4" xfId="343" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2787,6 +2817,9 @@
     <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="431" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="433" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="435" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="243" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -3001,6 +3034,9 @@
     <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="426" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="428" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="430" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="432" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="434" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="244" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3331,11 +3367,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J196"/>
+  <dimension ref="A1:J199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A193" sqref="A193:XFD193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5186,137 +5222,134 @@
         <v>410</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="12.75" customHeight="1">
+    <row r="163" spans="1:10" ht="24">
       <c r="A163" s="7"/>
       <c r="B163" t="s">
         <v>4</v>
       </c>
       <c r="D163" t="s">
-        <v>401</v>
+        <v>547</v>
       </c>
       <c r="E163" t="s">
-        <v>25</v>
-      </c>
-      <c r="I163" s="9"/>
+        <v>548</v>
+      </c>
     </row>
     <row r="164" spans="1:10" ht="12.75" customHeight="1">
       <c r="A164" s="7"/>
-      <c r="B164" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="B164" t="s">
+        <v>4</v>
+      </c>
+      <c r="D164" t="s">
+        <v>401</v>
+      </c>
+      <c r="E164" t="s">
+        <v>549</v>
+      </c>
+      <c r="I164" s="9"/>
     </row>
     <row r="165" spans="1:10" ht="12.75" customHeight="1">
       <c r="A165" s="7"/>
-      <c r="B165" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E165" t="s">
-        <v>26</v>
+      <c r="B165" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="166" spans="1:10" ht="12.75" customHeight="1">
       <c r="A166" s="7"/>
-      <c r="B166" t="s">
-        <v>23</v>
-      </c>
-      <c r="C166" t="s">
-        <v>27</v>
-      </c>
-      <c r="D166" t="s">
-        <v>411</v>
+      <c r="B166" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E166" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="167" spans="1:10" ht="12.75" customHeight="1">
       <c r="A167" s="7"/>
       <c r="B167" t="s">
+        <v>23</v>
+      </c>
+      <c r="C167" t="s">
+        <v>27</v>
+      </c>
+      <c r="D167" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" ht="24">
+      <c r="A168" s="7"/>
+      <c r="B168" t="s">
         <v>4</v>
       </c>
-      <c r="D167" t="s">
-        <v>402</v>
-      </c>
-      <c r="E167" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A168" s="7"/>
-      <c r="B168" s="11" t="s">
-        <v>15</v>
+      <c r="D168" t="s">
+        <v>547</v>
+      </c>
+      <c r="E168" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="169" spans="1:10" ht="12.75" customHeight="1">
       <c r="A169" s="7"/>
-      <c r="B169" s="11" t="s">
-        <v>15</v>
+      <c r="B169" t="s">
+        <v>4</v>
+      </c>
+      <c r="D169" t="s">
+        <v>402</v>
+      </c>
+      <c r="E169" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="170" spans="1:10" ht="12.75" customHeight="1">
       <c r="A170" s="7"/>
-      <c r="B170" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E170" t="s">
-        <v>61</v>
+      <c r="B170" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="171" spans="1:10" ht="12.75" customHeight="1">
       <c r="A171" s="7"/>
-      <c r="B171" t="s">
-        <v>4</v>
-      </c>
-      <c r="D171" t="s">
-        <v>62</v>
+      <c r="B171" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="172" spans="1:10" ht="12.75" customHeight="1">
       <c r="A172" s="7"/>
-      <c r="B172" t="s">
-        <v>23</v>
-      </c>
-      <c r="C172" t="s">
-        <v>63</v>
-      </c>
-      <c r="D172" t="s">
-        <v>412</v>
+      <c r="B172" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E172" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="173" spans="1:10" ht="12.75" customHeight="1">
       <c r="A173" s="7"/>
       <c r="B173" t="s">
-        <v>23</v>
-      </c>
-      <c r="C173" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="D173" t="s">
-        <v>413</v>
+        <v>62</v>
       </c>
     </row>
     <row r="174" spans="1:10" ht="12.75" customHeight="1">
       <c r="A174" s="7"/>
       <c r="B174" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="C174" t="s">
+        <v>63</v>
       </c>
       <c r="D174" t="s">
-        <v>539</v>
-      </c>
-      <c r="E174" t="s">
-        <v>538</v>
-      </c>
-      <c r="J174" t="s">
-        <v>535</v>
+        <v>412</v>
       </c>
     </row>
     <row r="175" spans="1:10" ht="12.75" customHeight="1">
       <c r="A175" s="7"/>
       <c r="B175" t="s">
-        <v>441</v>
+        <v>23</v>
+      </c>
+      <c r="C175" t="s">
+        <v>64</v>
       </c>
       <c r="D175" t="s">
-        <v>533</v>
-      </c>
-      <c r="E175" t="s">
-        <v>536</v>
+        <v>413</v>
       </c>
     </row>
     <row r="176" spans="1:10" ht="12.75" customHeight="1">
@@ -5325,188 +5358,227 @@
         <v>4</v>
       </c>
       <c r="D176" t="s">
-        <v>403</v>
+        <v>539</v>
       </c>
       <c r="E176" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="J176" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="12.75" customHeight="1">
+    <row r="177" spans="1:10" ht="12.75" customHeight="1">
       <c r="A177" s="7"/>
-      <c r="B177" s="11" t="s">
+      <c r="B177" t="s">
+        <v>441</v>
+      </c>
+      <c r="D177" t="s">
+        <v>533</v>
+      </c>
+      <c r="E177" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A178" s="7"/>
+      <c r="B178" t="s">
+        <v>4</v>
+      </c>
+      <c r="D178" t="s">
+        <v>403</v>
+      </c>
+      <c r="E178" t="s">
+        <v>537</v>
+      </c>
+      <c r="J178" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A179" s="7"/>
+      <c r="B179" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A178" s="7"/>
-      <c r="B178" s="10" t="s">
+    <row r="180" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A180" s="7"/>
+      <c r="B180" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E180" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A179" s="7"/>
-      <c r="B179" t="s">
-        <v>4</v>
-      </c>
-      <c r="D179" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A180" s="7"/>
-      <c r="B180" t="s">
-        <v>23</v>
-      </c>
-      <c r="C180" t="s">
-        <v>68</v>
-      </c>
-      <c r="D180" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" ht="12.75" customHeight="1">
+    <row r="181" spans="1:10" ht="12.75" customHeight="1">
       <c r="A181" s="7"/>
       <c r="B181" t="s">
-        <v>23</v>
-      </c>
-      <c r="C181" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="D181" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="12.75" customHeight="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" ht="12.75" customHeight="1">
       <c r="A182" s="7"/>
       <c r="B182" t="s">
+        <v>23</v>
+      </c>
+      <c r="C182" t="s">
+        <v>68</v>
+      </c>
+      <c r="D182" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A183" s="7"/>
+      <c r="B183" t="s">
+        <v>23</v>
+      </c>
+      <c r="C183" t="s">
+        <v>69</v>
+      </c>
+      <c r="D183" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A184" s="7"/>
+      <c r="B184" t="s">
         <v>4</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D184" t="s">
+        <v>552</v>
+      </c>
+      <c r="E184" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A185" s="7"/>
+      <c r="B185" t="s">
+        <v>4</v>
+      </c>
+      <c r="D185" t="s">
         <v>404</v>
       </c>
-      <c r="E182" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A183" s="7"/>
-      <c r="B183" s="11" t="s">
+      <c r="E185" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A186" s="7"/>
+      <c r="B186" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A184" s="7"/>
-      <c r="B184" s="10" t="s">
+    <row r="187" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A187" s="7"/>
+      <c r="B187" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E187" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A185" s="7"/>
-      <c r="B185" s="12" t="s">
+    <row r="188" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A188" s="7"/>
+      <c r="B188" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D188" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A186" s="7"/>
-      <c r="B186" t="s">
-        <v>41</v>
-      </c>
-      <c r="C186" t="s">
-        <v>48</v>
-      </c>
-      <c r="D186" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A187" s="7"/>
-      <c r="B187" t="s">
-        <v>4</v>
-      </c>
-      <c r="D187" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A188" s="7"/>
-      <c r="B188" t="s">
-        <v>42</v>
-      </c>
-      <c r="C188" t="s">
-        <v>43</v>
-      </c>
-      <c r="D188" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" ht="12.75" customHeight="1">
+    <row r="189" spans="1:10" ht="12.75" customHeight="1">
       <c r="A189" s="7"/>
       <c r="B189" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C189" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D189" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" ht="12.75" customHeight="1">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" ht="12.75" customHeight="1">
       <c r="A190" s="7"/>
       <c r="B190" t="s">
         <v>4</v>
       </c>
       <c r="D190" t="s">
-        <v>405</v>
-      </c>
-      <c r="E190" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" ht="12.75" customHeight="1">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" ht="12.75" customHeight="1">
       <c r="A191" s="7"/>
       <c r="B191" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="C191" t="s">
+        <v>43</v>
       </c>
       <c r="D191" t="s">
-        <v>406</v>
-      </c>
-      <c r="E191" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" ht="12.75" customHeight="1">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" ht="12.75" customHeight="1">
       <c r="A192" s="7"/>
-      <c r="B192" s="11" t="s">
-        <v>15</v>
+      <c r="B192" t="s">
+        <v>42</v>
+      </c>
+      <c r="C192" t="s">
+        <v>44</v>
+      </c>
+      <c r="D192" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="12.75" customHeight="1">
       <c r="A193" s="7"/>
-      <c r="B193" s="8" t="s">
+      <c r="B193" t="s">
+        <v>4</v>
+      </c>
+      <c r="D193" t="s">
+        <v>405</v>
+      </c>
+      <c r="E193" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A194" s="7"/>
+      <c r="B194" t="s">
+        <v>4</v>
+      </c>
+      <c r="D194" t="s">
+        <v>406</v>
+      </c>
+      <c r="E194" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A195" s="7"/>
+      <c r="B195" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A196" s="7"/>
+      <c r="B196" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C193" s="8"/>
-      <c r="D193" s="8"/>
-      <c r="E193" s="8"/>
-      <c r="F193" s="8"/>
-      <c r="G193" s="8"/>
-      <c r="H193" s="8"/>
-    </row>
-    <row r="196" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B196" s="34" t="s">
+      <c r="C196" s="8"/>
+      <c r="D196" s="8"/>
+      <c r="E196" s="8"/>
+      <c r="F196" s="8"/>
+      <c r="G196" s="8"/>
+      <c r="H196" s="8"/>
+    </row>
+    <row r="199" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B199" s="34" t="s">
         <v>377</v>
       </c>
     </row>

</xml_diff>